<commit_message>
Tuesday May 22 Update
</commit_message>
<xml_diff>
--- a/General/Curriculum (Personalized).xlsx
+++ b/General/Curriculum (Personalized).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13485" windowHeight="11415" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13485" windowHeight="11415" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Curriculum" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="991">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="1001">
   <si>
     <t>Week</t>
   </si>
@@ -10071,6 +10071,100 @@
   </si>
   <si>
     <t>No-SQL, SQL</t>
+  </si>
+  <si>
+    <t>https://angular.io/tutorial/toh-pt0</t>
+  </si>
+  <si>
+    <r>
+      <t>Components</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> are the fundamental building blocks of Angular applications. They display data on the screen, listen for user input, and take action based on that input.</t>
+    </r>
+  </si>
+  <si>
+    <t>Angular Components</t>
+  </si>
+  <si>
+    <r>
+      <t>You'll find the implementation of the shell </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF333333"/>
+        <rFont val="Droid Sans Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>AppComponent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> distributed over three files:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1. app.component.ts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>— the component class code, written in TypeScript.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2. app.component.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>— the component template, written in HTML.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3. app.component.css</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>— the component's private CSS styles.</t>
+    </r>
+  </si>
+  <si>
+    <t>Angular CLI</t>
+  </si>
+  <si>
+    <t>Angular now has its own CLI, or command line interface, which will do most of the routine operations for you.</t>
+  </si>
+  <si>
+    <t>https://www.toptal.com/angular/angular-5-tutorial</t>
   </si>
 </sst>
 </file>
@@ -10080,7 +10174,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="52">
+  <fonts count="55">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -10442,6 +10536,25 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Droid Sans Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="9">
@@ -11400,7 +11513,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="300">
+  <cellXfs count="303">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -11883,115 +11996,67 @@
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="37" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -11999,6 +12064,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -12009,55 +12089,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12078,71 +12128,116 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="37" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -12150,13 +12245,19 @@
     <xf numFmtId="0" fontId="14" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12168,20 +12269,29 @@
     <xf numFmtId="0" fontId="35" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -12189,10 +12299,13 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
@@ -12212,6 +12325,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -13231,21 +13353,21 @@
       <c r="H1" s="35" t="s">
         <v>193</v>
       </c>
-      <c r="I1" s="263" t="s">
+      <c r="I1" s="190" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="264"/>
-      <c r="K1" s="265"/>
-      <c r="L1" s="197" t="s">
+      <c r="J1" s="191"/>
+      <c r="K1" s="192"/>
+      <c r="L1" s="265" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="198"/>
+      <c r="M1" s="266"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A2" s="226">
+      <c r="A2" s="223">
         <v>1</v>
       </c>
-      <c r="B2" s="229" t="s">
+      <c r="B2" s="218" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -13254,145 +13376,145 @@
       <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="220" t="s">
+      <c r="E2" s="205" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="269"/>
-      <c r="G2" s="221"/>
-      <c r="H2" s="221"/>
-      <c r="I2" s="221" t="s">
+      <c r="F2" s="207"/>
+      <c r="G2" s="198"/>
+      <c r="H2" s="198"/>
+      <c r="I2" s="198" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="221" t="s">
+      <c r="J2" s="198" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="221" t="s">
+      <c r="K2" s="198" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="193" t="s">
+      <c r="L2" s="259" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="193" t="s">
+      <c r="M2" s="259" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A3" s="227"/>
-      <c r="B3" s="230"/>
+      <c r="A3" s="211"/>
+      <c r="B3" s="219"/>
       <c r="C3" s="32" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="215"/>
-      <c r="F3" s="242"/>
-      <c r="G3" s="212"/>
-      <c r="H3" s="212"/>
-      <c r="I3" s="212"/>
-      <c r="J3" s="212"/>
-      <c r="K3" s="212"/>
-      <c r="L3" s="190"/>
-      <c r="M3" s="190"/>
+      <c r="E3" s="200"/>
+      <c r="F3" s="208"/>
+      <c r="G3" s="194"/>
+      <c r="H3" s="194"/>
+      <c r="I3" s="194"/>
+      <c r="J3" s="194"/>
+      <c r="K3" s="194"/>
+      <c r="L3" s="242"/>
+      <c r="M3" s="242"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A4" s="227"/>
-      <c r="B4" s="230"/>
+      <c r="A4" s="211"/>
+      <c r="B4" s="219"/>
       <c r="C4" s="32" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="215"/>
-      <c r="F4" s="242"/>
-      <c r="G4" s="212"/>
-      <c r="H4" s="212"/>
-      <c r="I4" s="212"/>
-      <c r="J4" s="212"/>
-      <c r="K4" s="212"/>
-      <c r="L4" s="190"/>
-      <c r="M4" s="190"/>
+      <c r="E4" s="200"/>
+      <c r="F4" s="208"/>
+      <c r="G4" s="194"/>
+      <c r="H4" s="194"/>
+      <c r="I4" s="194"/>
+      <c r="J4" s="194"/>
+      <c r="K4" s="194"/>
+      <c r="L4" s="242"/>
+      <c r="M4" s="242"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A5" s="227"/>
-      <c r="B5" s="230"/>
+      <c r="A5" s="211"/>
+      <c r="B5" s="219"/>
       <c r="C5" s="32" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="215"/>
-      <c r="F5" s="242"/>
-      <c r="G5" s="212"/>
-      <c r="H5" s="212"/>
-      <c r="I5" s="212"/>
-      <c r="J5" s="212"/>
-      <c r="K5" s="212"/>
-      <c r="L5" s="190"/>
-      <c r="M5" s="190"/>
+      <c r="E5" s="200"/>
+      <c r="F5" s="208"/>
+      <c r="G5" s="194"/>
+      <c r="H5" s="194"/>
+      <c r="I5" s="194"/>
+      <c r="J5" s="194"/>
+      <c r="K5" s="194"/>
+      <c r="L5" s="242"/>
+      <c r="M5" s="242"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A6" s="227"/>
-      <c r="B6" s="230"/>
+      <c r="A6" s="211"/>
+      <c r="B6" s="219"/>
       <c r="C6" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="215"/>
-      <c r="F6" s="242"/>
-      <c r="G6" s="212"/>
-      <c r="H6" s="212"/>
-      <c r="I6" s="212"/>
-      <c r="J6" s="212"/>
-      <c r="K6" s="212"/>
-      <c r="L6" s="190"/>
-      <c r="M6" s="190"/>
+      <c r="E6" s="200"/>
+      <c r="F6" s="208"/>
+      <c r="G6" s="194"/>
+      <c r="H6" s="194"/>
+      <c r="I6" s="194"/>
+      <c r="J6" s="194"/>
+      <c r="K6" s="194"/>
+      <c r="L6" s="242"/>
+      <c r="M6" s="242"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A7" s="227"/>
-      <c r="B7" s="230"/>
+      <c r="A7" s="211"/>
+      <c r="B7" s="219"/>
       <c r="C7" s="32" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="215"/>
-      <c r="F7" s="242"/>
-      <c r="G7" s="212"/>
-      <c r="H7" s="212"/>
-      <c r="I7" s="212"/>
-      <c r="J7" s="212"/>
-      <c r="K7" s="212"/>
-      <c r="L7" s="190"/>
-      <c r="M7" s="190"/>
+      <c r="E7" s="200"/>
+      <c r="F7" s="208"/>
+      <c r="G7" s="194"/>
+      <c r="H7" s="194"/>
+      <c r="I7" s="194"/>
+      <c r="J7" s="194"/>
+      <c r="K7" s="194"/>
+      <c r="L7" s="242"/>
+      <c r="M7" s="242"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A8" s="228"/>
-      <c r="B8" s="231"/>
+      <c r="A8" s="212"/>
+      <c r="B8" s="220"/>
       <c r="C8" s="9" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="268"/>
-      <c r="F8" s="270"/>
-      <c r="G8" s="267"/>
-      <c r="H8" s="267"/>
-      <c r="I8" s="267"/>
-      <c r="J8" s="267"/>
-      <c r="K8" s="267"/>
-      <c r="L8" s="203"/>
-      <c r="M8" s="203"/>
+      <c r="E8" s="206"/>
+      <c r="F8" s="209"/>
+      <c r="G8" s="199"/>
+      <c r="H8" s="199"/>
+      <c r="I8" s="199"/>
+      <c r="J8" s="199"/>
+      <c r="K8" s="199"/>
+      <c r="L8" s="268"/>
+      <c r="M8" s="268"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A9" s="233">
+      <c r="A9" s="236">
         <v>2</v>
       </c>
-      <c r="B9" s="229" t="s">
+      <c r="B9" s="218" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -13401,864 +13523,864 @@
       <c r="D9" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="E9" s="246"/>
-      <c r="F9" s="225" t="s">
+      <c r="E9" s="201"/>
+      <c r="F9" s="202" t="s">
         <v>192</v>
       </c>
-      <c r="G9" s="240" t="s">
+      <c r="G9" s="204" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="224"/>
-      <c r="I9" s="244" t="s">
+      <c r="H9" s="245"/>
+      <c r="I9" s="246" t="s">
         <v>184</v>
       </c>
-      <c r="J9" s="225" t="s">
+      <c r="J9" s="202" t="s">
         <v>194</v>
       </c>
-      <c r="K9" s="225" t="s">
+      <c r="K9" s="202" t="s">
         <v>195</v>
       </c>
-      <c r="L9" s="240" t="s">
+      <c r="L9" s="204" t="s">
         <v>328</v>
       </c>
-      <c r="M9" s="204"/>
+      <c r="M9" s="269"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1">
       <c r="A10" s="234"/>
-      <c r="B10" s="230"/>
+      <c r="B10" s="219"/>
       <c r="C10" s="11" t="s">
         <v>26</v>
       </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="207"/>
-      <c r="F10" s="214"/>
-      <c r="G10" s="218"/>
-      <c r="H10" s="210"/>
-      <c r="I10" s="245"/>
-      <c r="J10" s="214"/>
-      <c r="K10" s="214"/>
-      <c r="L10" s="241"/>
-      <c r="M10" s="205"/>
+      <c r="E10" s="193"/>
+      <c r="F10" s="203"/>
+      <c r="G10" s="196"/>
+      <c r="H10" s="197"/>
+      <c r="I10" s="247"/>
+      <c r="J10" s="203"/>
+      <c r="K10" s="203"/>
+      <c r="L10" s="240"/>
+      <c r="M10" s="270"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A11" s="252">
+      <c r="A11" s="231">
         <v>3</v>
       </c>
-      <c r="B11" s="230"/>
+      <c r="B11" s="219"/>
       <c r="C11" s="11" t="s">
         <v>263</v>
       </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="215"/>
-      <c r="F11" s="242"/>
-      <c r="G11" s="212"/>
-      <c r="H11" s="212" t="s">
+      <c r="E11" s="200"/>
+      <c r="F11" s="208"/>
+      <c r="G11" s="194"/>
+      <c r="H11" s="194" t="s">
         <v>198</v>
       </c>
-      <c r="I11" s="212" t="s">
+      <c r="I11" s="194" t="s">
         <v>196</v>
       </c>
-      <c r="J11" s="212"/>
-      <c r="K11" s="212"/>
+      <c r="J11" s="194"/>
+      <c r="K11" s="194"/>
       <c r="L11" s="239" t="s">
         <v>329</v>
       </c>
-      <c r="M11" s="190"/>
+      <c r="M11" s="242"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A12" s="253"/>
-      <c r="B12" s="230"/>
+      <c r="A12" s="232"/>
+      <c r="B12" s="219"/>
       <c r="C12" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D12" s="10"/>
-      <c r="E12" s="215"/>
-      <c r="F12" s="242"/>
-      <c r="G12" s="212"/>
-      <c r="H12" s="212"/>
-      <c r="I12" s="212"/>
-      <c r="J12" s="212"/>
-      <c r="K12" s="212"/>
+      <c r="E12" s="200"/>
+      <c r="F12" s="208"/>
+      <c r="G12" s="194"/>
+      <c r="H12" s="194"/>
+      <c r="I12" s="194"/>
+      <c r="J12" s="194"/>
+      <c r="K12" s="194"/>
       <c r="L12" s="239"/>
-      <c r="M12" s="190"/>
+      <c r="M12" s="242"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A13" s="254">
+      <c r="A13" s="233">
         <v>4</v>
       </c>
-      <c r="B13" s="230"/>
+      <c r="B13" s="219"/>
       <c r="C13" s="11" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="11"/>
-      <c r="E13" s="207"/>
-      <c r="F13" s="266" t="s">
+      <c r="E13" s="193"/>
+      <c r="F13" s="195" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="218" t="s">
+      <c r="G13" s="196" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="210"/>
-      <c r="I13" s="218" t="s">
+      <c r="H13" s="197"/>
+      <c r="I13" s="196" t="s">
         <v>330</v>
       </c>
-      <c r="J13" s="210"/>
-      <c r="K13" s="210"/>
-      <c r="L13" s="191"/>
-      <c r="M13" s="191"/>
+      <c r="J13" s="197"/>
+      <c r="K13" s="197"/>
+      <c r="L13" s="260"/>
+      <c r="M13" s="260"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1">
       <c r="A14" s="234"/>
-      <c r="B14" s="230"/>
+      <c r="B14" s="219"/>
       <c r="C14" s="32" t="s">
         <v>30</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="207"/>
-      <c r="F14" s="266"/>
-      <c r="G14" s="218"/>
-      <c r="H14" s="210"/>
-      <c r="I14" s="218"/>
-      <c r="J14" s="210"/>
-      <c r="K14" s="210"/>
-      <c r="L14" s="191"/>
-      <c r="M14" s="191"/>
+      <c r="E14" s="193"/>
+      <c r="F14" s="195"/>
+      <c r="G14" s="196"/>
+      <c r="H14" s="197"/>
+      <c r="I14" s="196"/>
+      <c r="J14" s="197"/>
+      <c r="K14" s="197"/>
+      <c r="L14" s="260"/>
+      <c r="M14" s="260"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A15" s="252">
+      <c r="A15" s="231">
         <v>5</v>
       </c>
-      <c r="B15" s="230"/>
+      <c r="B15" s="219"/>
       <c r="C15" s="237" t="s">
         <v>31</v>
       </c>
       <c r="D15" s="4"/>
-      <c r="E15" s="215" t="s">
+      <c r="E15" s="200" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="242"/>
-      <c r="G15" s="212"/>
-      <c r="H15" s="212"/>
-      <c r="I15" s="212"/>
-      <c r="J15" s="212"/>
-      <c r="K15" s="212"/>
-      <c r="L15" s="190"/>
-      <c r="M15" s="190"/>
+      <c r="F15" s="208"/>
+      <c r="G15" s="194"/>
+      <c r="H15" s="194"/>
+      <c r="I15" s="194"/>
+      <c r="J15" s="194"/>
+      <c r="K15" s="194"/>
+      <c r="L15" s="242"/>
+      <c r="M15" s="242"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A16" s="255"/>
-      <c r="B16" s="232"/>
+      <c r="A16" s="235"/>
+      <c r="B16" s="224"/>
       <c r="C16" s="238"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="216"/>
-      <c r="F16" s="243"/>
-      <c r="G16" s="213"/>
-      <c r="H16" s="213"/>
-      <c r="I16" s="213"/>
-      <c r="J16" s="213"/>
-      <c r="K16" s="213"/>
-      <c r="L16" s="195"/>
-      <c r="M16" s="195"/>
+      <c r="E16" s="248"/>
+      <c r="F16" s="244"/>
+      <c r="G16" s="241"/>
+      <c r="H16" s="241"/>
+      <c r="I16" s="241"/>
+      <c r="J16" s="241"/>
+      <c r="K16" s="241"/>
+      <c r="L16" s="243"/>
+      <c r="M16" s="243"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A17" s="256">
+      <c r="A17" s="221">
         <v>6</v>
       </c>
-      <c r="B17" s="229" t="s">
+      <c r="B17" s="218" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>35</v>
       </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="246"/>
-      <c r="F17" s="224"/>
-      <c r="G17" s="224"/>
-      <c r="H17" s="225" t="s">
+      <c r="E17" s="201"/>
+      <c r="F17" s="245"/>
+      <c r="G17" s="245"/>
+      <c r="H17" s="202" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="225"/>
-      <c r="J17" s="225"/>
-      <c r="K17" s="225"/>
-      <c r="L17" s="199"/>
-      <c r="M17" s="199"/>
+      <c r="I17" s="202"/>
+      <c r="J17" s="202"/>
+      <c r="K17" s="202"/>
+      <c r="L17" s="267"/>
+      <c r="M17" s="267"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A18" s="235"/>
-      <c r="B18" s="230"/>
+      <c r="A18" s="210"/>
+      <c r="B18" s="219"/>
       <c r="C18" s="11" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="4"/>
-      <c r="E18" s="207"/>
-      <c r="F18" s="210"/>
-      <c r="G18" s="210"/>
-      <c r="H18" s="214"/>
-      <c r="I18" s="214"/>
-      <c r="J18" s="214"/>
-      <c r="K18" s="214"/>
-      <c r="L18" s="194"/>
-      <c r="M18" s="194"/>
+      <c r="E18" s="193"/>
+      <c r="F18" s="197"/>
+      <c r="G18" s="197"/>
+      <c r="H18" s="203"/>
+      <c r="I18" s="203"/>
+      <c r="J18" s="203"/>
+      <c r="K18" s="203"/>
+      <c r="L18" s="253"/>
+      <c r="M18" s="253"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A19" s="235"/>
-      <c r="B19" s="230"/>
+      <c r="A19" s="210"/>
+      <c r="B19" s="219"/>
       <c r="C19" s="11" t="s">
         <v>38</v>
       </c>
       <c r="D19" s="4"/>
-      <c r="E19" s="207"/>
-      <c r="F19" s="210"/>
-      <c r="G19" s="210"/>
-      <c r="H19" s="214"/>
-      <c r="I19" s="214"/>
-      <c r="J19" s="214"/>
-      <c r="K19" s="214"/>
-      <c r="L19" s="194"/>
-      <c r="M19" s="194"/>
+      <c r="E19" s="193"/>
+      <c r="F19" s="197"/>
+      <c r="G19" s="197"/>
+      <c r="H19" s="203"/>
+      <c r="I19" s="203"/>
+      <c r="J19" s="203"/>
+      <c r="K19" s="203"/>
+      <c r="L19" s="253"/>
+      <c r="M19" s="253"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A20" s="227">
+      <c r="A20" s="211">
         <v>7</v>
       </c>
-      <c r="B20" s="230"/>
+      <c r="B20" s="219"/>
       <c r="C20" s="11" t="s">
         <v>39</v>
       </c>
       <c r="D20" s="4"/>
-      <c r="E20" s="215" t="s">
+      <c r="E20" s="200" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="223" t="s">
+      <c r="F20" s="255" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="223"/>
-      <c r="H20" s="223"/>
-      <c r="I20" s="223"/>
-      <c r="J20" s="223"/>
-      <c r="K20" s="223"/>
-      <c r="L20" s="200"/>
-      <c r="M20" s="200"/>
+      <c r="G20" s="255"/>
+      <c r="H20" s="255"/>
+      <c r="I20" s="255"/>
+      <c r="J20" s="255"/>
+      <c r="K20" s="255"/>
+      <c r="L20" s="256"/>
+      <c r="M20" s="256"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A21" s="227"/>
-      <c r="B21" s="230"/>
+      <c r="A21" s="211"/>
+      <c r="B21" s="219"/>
       <c r="C21" s="11" t="s">
         <v>41</v>
       </c>
       <c r="D21" s="4"/>
-      <c r="E21" s="215"/>
-      <c r="F21" s="223"/>
-      <c r="G21" s="223"/>
-      <c r="H21" s="223"/>
-      <c r="I21" s="223"/>
-      <c r="J21" s="223"/>
-      <c r="K21" s="223"/>
-      <c r="L21" s="200"/>
-      <c r="M21" s="200"/>
+      <c r="E21" s="200"/>
+      <c r="F21" s="255"/>
+      <c r="G21" s="255"/>
+      <c r="H21" s="255"/>
+      <c r="I21" s="255"/>
+      <c r="J21" s="255"/>
+      <c r="K21" s="255"/>
+      <c r="L21" s="256"/>
+      <c r="M21" s="256"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A22" s="227"/>
-      <c r="B22" s="230"/>
+      <c r="A22" s="211"/>
+      <c r="B22" s="219"/>
       <c r="C22" s="32" t="s">
         <v>42</v>
       </c>
       <c r="D22" s="4"/>
-      <c r="E22" s="215"/>
-      <c r="F22" s="223"/>
-      <c r="G22" s="223"/>
-      <c r="H22" s="223"/>
-      <c r="I22" s="223"/>
-      <c r="J22" s="223"/>
-      <c r="K22" s="223"/>
-      <c r="L22" s="200"/>
-      <c r="M22" s="200"/>
+      <c r="E22" s="200"/>
+      <c r="F22" s="255"/>
+      <c r="G22" s="255"/>
+      <c r="H22" s="255"/>
+      <c r="I22" s="255"/>
+      <c r="J22" s="255"/>
+      <c r="K22" s="255"/>
+      <c r="L22" s="256"/>
+      <c r="M22" s="256"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A23" s="235">
+      <c r="A23" s="210">
         <v>8</v>
       </c>
-      <c r="B23" s="230"/>
+      <c r="B23" s="219"/>
       <c r="C23" s="32" t="s">
         <v>43</v>
       </c>
       <c r="D23" s="4"/>
-      <c r="E23" s="207"/>
-      <c r="F23" s="210"/>
-      <c r="G23" s="218" t="s">
+      <c r="E23" s="193"/>
+      <c r="F23" s="197"/>
+      <c r="G23" s="196" t="s">
         <v>50</v>
       </c>
-      <c r="H23" s="214" t="s">
+      <c r="H23" s="203" t="s">
         <v>32</v>
       </c>
-      <c r="I23" s="214"/>
-      <c r="J23" s="214"/>
-      <c r="K23" s="214"/>
-      <c r="L23" s="194"/>
-      <c r="M23" s="194"/>
+      <c r="I23" s="203"/>
+      <c r="J23" s="203"/>
+      <c r="K23" s="203"/>
+      <c r="L23" s="253"/>
+      <c r="M23" s="253"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A24" s="235"/>
-      <c r="B24" s="230"/>
+      <c r="A24" s="210"/>
+      <c r="B24" s="219"/>
       <c r="C24" s="32" t="s">
         <v>45</v>
       </c>
       <c r="D24" s="4"/>
-      <c r="E24" s="207"/>
-      <c r="F24" s="210"/>
-      <c r="G24" s="218"/>
-      <c r="H24" s="214"/>
-      <c r="I24" s="214"/>
-      <c r="J24" s="214"/>
-      <c r="K24" s="214"/>
-      <c r="L24" s="194"/>
-      <c r="M24" s="194"/>
+      <c r="E24" s="193"/>
+      <c r="F24" s="197"/>
+      <c r="G24" s="196"/>
+      <c r="H24" s="203"/>
+      <c r="I24" s="203"/>
+      <c r="J24" s="203"/>
+      <c r="K24" s="203"/>
+      <c r="L24" s="253"/>
+      <c r="M24" s="253"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A25" s="236"/>
-      <c r="B25" s="232"/>
+      <c r="A25" s="227"/>
+      <c r="B25" s="224"/>
       <c r="C25" s="33" t="s">
         <v>46</v>
       </c>
       <c r="D25" s="5"/>
-      <c r="E25" s="208"/>
-      <c r="F25" s="211"/>
-      <c r="G25" s="219"/>
-      <c r="H25" s="217"/>
-      <c r="I25" s="217"/>
-      <c r="J25" s="217"/>
-      <c r="K25" s="217"/>
-      <c r="L25" s="201"/>
-      <c r="M25" s="201"/>
+      <c r="E25" s="249"/>
+      <c r="F25" s="250"/>
+      <c r="G25" s="251"/>
+      <c r="H25" s="252"/>
+      <c r="I25" s="252"/>
+      <c r="J25" s="252"/>
+      <c r="K25" s="252"/>
+      <c r="L25" s="254"/>
+      <c r="M25" s="254"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A26" s="247">
+      <c r="A26" s="225">
         <v>9</v>
       </c>
-      <c r="B26" s="229" t="s">
+      <c r="B26" s="218" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>48</v>
       </c>
       <c r="D26" s="3"/>
-      <c r="E26" s="220" t="s">
+      <c r="E26" s="205" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="222" t="s">
+      <c r="F26" s="257" t="s">
         <v>53</v>
       </c>
-      <c r="G26" s="222"/>
-      <c r="H26" s="222"/>
-      <c r="I26" s="222"/>
-      <c r="J26" s="222"/>
-      <c r="K26" s="222"/>
-      <c r="L26" s="202"/>
-      <c r="M26" s="202"/>
+      <c r="G26" s="257"/>
+      <c r="H26" s="257"/>
+      <c r="I26" s="257"/>
+      <c r="J26" s="257"/>
+      <c r="K26" s="257"/>
+      <c r="L26" s="258"/>
+      <c r="M26" s="258"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A27" s="248"/>
-      <c r="B27" s="230"/>
+      <c r="A27" s="226"/>
+      <c r="B27" s="219"/>
       <c r="C27" s="13" t="s">
         <v>51</v>
       </c>
       <c r="D27" s="4"/>
-      <c r="E27" s="215"/>
-      <c r="F27" s="223"/>
-      <c r="G27" s="223"/>
-      <c r="H27" s="223"/>
-      <c r="I27" s="223"/>
-      <c r="J27" s="223"/>
-      <c r="K27" s="223"/>
-      <c r="L27" s="200"/>
-      <c r="M27" s="200"/>
+      <c r="E27" s="200"/>
+      <c r="F27" s="255"/>
+      <c r="G27" s="255"/>
+      <c r="H27" s="255"/>
+      <c r="I27" s="255"/>
+      <c r="J27" s="255"/>
+      <c r="K27" s="255"/>
+      <c r="L27" s="256"/>
+      <c r="M27" s="256"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A28" s="236">
+      <c r="A28" s="227">
         <v>10</v>
       </c>
-      <c r="B28" s="230"/>
+      <c r="B28" s="219"/>
       <c r="C28" s="13" t="s">
         <v>52</v>
       </c>
       <c r="D28" s="4"/>
-      <c r="E28" s="207"/>
-      <c r="F28" s="214" t="s">
+      <c r="E28" s="193"/>
+      <c r="F28" s="203" t="s">
         <v>59</v>
       </c>
-      <c r="G28" s="214"/>
-      <c r="H28" s="214" t="s">
+      <c r="G28" s="203"/>
+      <c r="H28" s="203" t="s">
         <v>40</v>
       </c>
-      <c r="I28" s="214"/>
-      <c r="J28" s="214"/>
-      <c r="K28" s="214"/>
-      <c r="L28" s="194"/>
-      <c r="M28" s="194"/>
+      <c r="I28" s="203"/>
+      <c r="J28" s="203"/>
+      <c r="K28" s="203"/>
+      <c r="L28" s="253"/>
+      <c r="M28" s="253"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A29" s="249"/>
-      <c r="B29" s="230"/>
+      <c r="A29" s="228"/>
+      <c r="B29" s="219"/>
       <c r="C29" s="13" t="s">
         <v>54</v>
       </c>
       <c r="D29" s="4"/>
-      <c r="E29" s="207"/>
-      <c r="F29" s="214"/>
-      <c r="G29" s="214"/>
-      <c r="H29" s="214"/>
-      <c r="I29" s="214"/>
-      <c r="J29" s="214"/>
-      <c r="K29" s="214"/>
-      <c r="L29" s="194"/>
-      <c r="M29" s="194"/>
+      <c r="E29" s="193"/>
+      <c r="F29" s="203"/>
+      <c r="G29" s="203"/>
+      <c r="H29" s="203"/>
+      <c r="I29" s="203"/>
+      <c r="J29" s="203"/>
+      <c r="K29" s="203"/>
+      <c r="L29" s="253"/>
+      <c r="M29" s="253"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A30" s="250">
+      <c r="A30" s="229">
         <v>11</v>
       </c>
-      <c r="B30" s="230"/>
+      <c r="B30" s="219"/>
       <c r="C30" s="13" t="s">
         <v>55</v>
       </c>
       <c r="D30" s="4"/>
-      <c r="E30" s="215" t="s">
+      <c r="E30" s="200" t="s">
         <v>49</v>
       </c>
-      <c r="F30" s="212"/>
-      <c r="G30" s="212"/>
-      <c r="H30" s="212"/>
-      <c r="I30" s="212"/>
-      <c r="J30" s="212"/>
-      <c r="K30" s="212"/>
-      <c r="L30" s="190"/>
-      <c r="M30" s="190"/>
+      <c r="F30" s="194"/>
+      <c r="G30" s="194"/>
+      <c r="H30" s="194"/>
+      <c r="I30" s="194"/>
+      <c r="J30" s="194"/>
+      <c r="K30" s="194"/>
+      <c r="L30" s="242"/>
+      <c r="M30" s="242"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A31" s="248"/>
-      <c r="B31" s="230"/>
+      <c r="A31" s="226"/>
+      <c r="B31" s="219"/>
       <c r="C31" s="14" t="s">
         <v>57</v>
       </c>
       <c r="D31" s="4"/>
-      <c r="E31" s="215"/>
-      <c r="F31" s="212"/>
-      <c r="G31" s="212"/>
-      <c r="H31" s="212"/>
-      <c r="I31" s="212"/>
-      <c r="J31" s="212"/>
-      <c r="K31" s="212"/>
-      <c r="L31" s="190"/>
-      <c r="M31" s="190"/>
+      <c r="E31" s="200"/>
+      <c r="F31" s="194"/>
+      <c r="G31" s="194"/>
+      <c r="H31" s="194"/>
+      <c r="I31" s="194"/>
+      <c r="J31" s="194"/>
+      <c r="K31" s="194"/>
+      <c r="L31" s="242"/>
+      <c r="M31" s="242"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A32" s="236">
+      <c r="A32" s="227">
         <v>12</v>
       </c>
-      <c r="B32" s="230"/>
+      <c r="B32" s="219"/>
       <c r="C32" s="14" t="s">
         <v>58</v>
       </c>
       <c r="D32" s="4"/>
-      <c r="E32" s="207"/>
-      <c r="F32" s="214" t="s">
+      <c r="E32" s="193"/>
+      <c r="F32" s="203" t="s">
         <v>67</v>
       </c>
-      <c r="G32" s="218" t="s">
+      <c r="G32" s="196" t="s">
         <v>64</v>
       </c>
-      <c r="H32" s="214" t="s">
+      <c r="H32" s="203" t="s">
         <v>49</v>
       </c>
-      <c r="I32" s="214"/>
-      <c r="J32" s="214"/>
-      <c r="K32" s="214"/>
-      <c r="L32" s="194"/>
-      <c r="M32" s="194"/>
+      <c r="I32" s="203"/>
+      <c r="J32" s="203"/>
+      <c r="K32" s="203"/>
+      <c r="L32" s="253"/>
+      <c r="M32" s="253"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A33" s="251"/>
-      <c r="B33" s="232"/>
+      <c r="A33" s="230"/>
+      <c r="B33" s="224"/>
       <c r="C33" s="15" t="s">
         <v>60</v>
       </c>
       <c r="D33" s="5"/>
-      <c r="E33" s="208"/>
-      <c r="F33" s="217"/>
-      <c r="G33" s="219"/>
-      <c r="H33" s="217"/>
-      <c r="I33" s="217"/>
-      <c r="J33" s="217"/>
-      <c r="K33" s="217"/>
-      <c r="L33" s="201"/>
-      <c r="M33" s="201"/>
+      <c r="E33" s="249"/>
+      <c r="F33" s="252"/>
+      <c r="G33" s="251"/>
+      <c r="H33" s="252"/>
+      <c r="I33" s="252"/>
+      <c r="J33" s="252"/>
+      <c r="K33" s="252"/>
+      <c r="L33" s="254"/>
+      <c r="M33" s="254"/>
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A34" s="226">
+      <c r="A34" s="223">
         <v>13</v>
       </c>
-      <c r="B34" s="229" t="s">
+      <c r="B34" s="218" t="s">
         <v>61</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>62</v>
       </c>
       <c r="D34" s="3"/>
-      <c r="E34" s="220" t="s">
+      <c r="E34" s="205" t="s">
         <v>56</v>
       </c>
-      <c r="F34" s="221"/>
-      <c r="G34" s="221"/>
-      <c r="H34" s="221"/>
-      <c r="I34" s="221"/>
-      <c r="J34" s="221"/>
-      <c r="K34" s="221"/>
-      <c r="L34" s="193"/>
-      <c r="M34" s="193"/>
+      <c r="F34" s="198"/>
+      <c r="G34" s="198"/>
+      <c r="H34" s="198"/>
+      <c r="I34" s="198"/>
+      <c r="J34" s="198"/>
+      <c r="K34" s="198"/>
+      <c r="L34" s="259"/>
+      <c r="M34" s="259"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A35" s="227"/>
-      <c r="B35" s="230"/>
+      <c r="A35" s="211"/>
+      <c r="B35" s="219"/>
       <c r="C35" s="17" t="s">
         <v>65</v>
       </c>
       <c r="D35" s="4"/>
-      <c r="E35" s="215"/>
-      <c r="F35" s="212"/>
-      <c r="G35" s="212"/>
-      <c r="H35" s="212"/>
-      <c r="I35" s="212"/>
-      <c r="J35" s="212"/>
-      <c r="K35" s="212"/>
-      <c r="L35" s="190"/>
-      <c r="M35" s="190"/>
+      <c r="E35" s="200"/>
+      <c r="F35" s="194"/>
+      <c r="G35" s="194"/>
+      <c r="H35" s="194"/>
+      <c r="I35" s="194"/>
+      <c r="J35" s="194"/>
+      <c r="K35" s="194"/>
+      <c r="L35" s="242"/>
+      <c r="M35" s="242"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A36" s="235">
+      <c r="A36" s="210">
         <v>14</v>
       </c>
-      <c r="B36" s="230"/>
+      <c r="B36" s="219"/>
       <c r="C36" s="17" t="s">
         <v>66</v>
       </c>
       <c r="D36" s="4"/>
-      <c r="E36" s="207"/>
-      <c r="F36" s="210" t="s">
+      <c r="E36" s="193"/>
+      <c r="F36" s="197" t="s">
         <v>73</v>
       </c>
-      <c r="G36" s="210"/>
-      <c r="H36" s="210" t="s">
+      <c r="G36" s="197"/>
+      <c r="H36" s="197" t="s">
         <v>56</v>
       </c>
-      <c r="I36" s="210"/>
-      <c r="J36" s="210"/>
-      <c r="K36" s="210"/>
-      <c r="L36" s="191"/>
-      <c r="M36" s="191"/>
+      <c r="I36" s="197"/>
+      <c r="J36" s="197"/>
+      <c r="K36" s="197"/>
+      <c r="L36" s="260"/>
+      <c r="M36" s="260"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A37" s="235"/>
-      <c r="B37" s="230"/>
+      <c r="A37" s="210"/>
+      <c r="B37" s="219"/>
       <c r="C37" s="17" t="s">
         <v>68</v>
       </c>
       <c r="D37" s="4"/>
-      <c r="E37" s="207"/>
-      <c r="F37" s="210"/>
-      <c r="G37" s="210"/>
-      <c r="H37" s="210"/>
-      <c r="I37" s="210"/>
-      <c r="J37" s="210"/>
-      <c r="K37" s="210"/>
-      <c r="L37" s="191"/>
-      <c r="M37" s="191"/>
+      <c r="E37" s="193"/>
+      <c r="F37" s="197"/>
+      <c r="G37" s="197"/>
+      <c r="H37" s="197"/>
+      <c r="I37" s="197"/>
+      <c r="J37" s="197"/>
+      <c r="K37" s="197"/>
+      <c r="L37" s="260"/>
+      <c r="M37" s="260"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A38" s="227">
+      <c r="A38" s="211">
         <v>15</v>
       </c>
-      <c r="B38" s="230"/>
+      <c r="B38" s="219"/>
       <c r="C38" s="17" t="s">
         <v>69</v>
       </c>
       <c r="D38" s="4"/>
-      <c r="E38" s="215" t="s">
+      <c r="E38" s="200" t="s">
         <v>63</v>
       </c>
-      <c r="F38" s="212"/>
-      <c r="G38" s="212"/>
-      <c r="H38" s="212"/>
-      <c r="I38" s="212"/>
-      <c r="J38" s="212"/>
-      <c r="K38" s="212"/>
-      <c r="L38" s="190"/>
-      <c r="M38" s="190"/>
+      <c r="F38" s="194"/>
+      <c r="G38" s="194"/>
+      <c r="H38" s="194"/>
+      <c r="I38" s="194"/>
+      <c r="J38" s="194"/>
+      <c r="K38" s="194"/>
+      <c r="L38" s="242"/>
+      <c r="M38" s="242"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A39" s="227"/>
-      <c r="B39" s="230"/>
+      <c r="A39" s="211"/>
+      <c r="B39" s="219"/>
       <c r="C39" s="32" t="s">
         <v>71</v>
       </c>
       <c r="D39" s="4"/>
-      <c r="E39" s="215"/>
-      <c r="F39" s="212"/>
-      <c r="G39" s="212"/>
-      <c r="H39" s="212"/>
-      <c r="I39" s="212"/>
-      <c r="J39" s="212"/>
-      <c r="K39" s="212"/>
-      <c r="L39" s="190"/>
-      <c r="M39" s="190"/>
+      <c r="E39" s="200"/>
+      <c r="F39" s="194"/>
+      <c r="G39" s="194"/>
+      <c r="H39" s="194"/>
+      <c r="I39" s="194"/>
+      <c r="J39" s="194"/>
+      <c r="K39" s="194"/>
+      <c r="L39" s="242"/>
+      <c r="M39" s="242"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A40" s="235">
+      <c r="A40" s="210">
         <v>16</v>
       </c>
-      <c r="B40" s="230"/>
+      <c r="B40" s="219"/>
       <c r="C40" s="32" t="s">
         <v>72</v>
       </c>
       <c r="D40" s="4"/>
-      <c r="E40" s="207"/>
-      <c r="F40" s="214" t="s">
+      <c r="E40" s="193"/>
+      <c r="F40" s="203" t="s">
         <v>82</v>
       </c>
-      <c r="G40" s="218" t="s">
+      <c r="G40" s="196" t="s">
         <v>79</v>
       </c>
-      <c r="H40" s="210" t="s">
+      <c r="H40" s="197" t="s">
         <v>63</v>
       </c>
-      <c r="I40" s="210"/>
-      <c r="J40" s="210"/>
-      <c r="K40" s="210"/>
-      <c r="L40" s="191"/>
-      <c r="M40" s="191"/>
+      <c r="I40" s="197"/>
+      <c r="J40" s="197"/>
+      <c r="K40" s="197"/>
+      <c r="L40" s="260"/>
+      <c r="M40" s="260"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A41" s="235"/>
-      <c r="B41" s="230"/>
+      <c r="A41" s="210"/>
+      <c r="B41" s="219"/>
       <c r="C41" s="32" t="s">
         <v>74</v>
       </c>
       <c r="D41" s="4"/>
-      <c r="E41" s="207"/>
-      <c r="F41" s="214"/>
-      <c r="G41" s="218"/>
-      <c r="H41" s="210"/>
-      <c r="I41" s="210"/>
-      <c r="J41" s="210"/>
-      <c r="K41" s="210"/>
-      <c r="L41" s="191"/>
-      <c r="M41" s="191"/>
+      <c r="E41" s="193"/>
+      <c r="F41" s="203"/>
+      <c r="G41" s="196"/>
+      <c r="H41" s="197"/>
+      <c r="I41" s="197"/>
+      <c r="J41" s="197"/>
+      <c r="K41" s="197"/>
+      <c r="L41" s="260"/>
+      <c r="M41" s="260"/>
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A42" s="262"/>
-      <c r="B42" s="231"/>
+      <c r="A42" s="222"/>
+      <c r="B42" s="220"/>
       <c r="C42" s="9" t="s">
         <v>75</v>
       </c>
       <c r="D42" s="5"/>
-      <c r="E42" s="208"/>
-      <c r="F42" s="217"/>
-      <c r="G42" s="219"/>
-      <c r="H42" s="211"/>
-      <c r="I42" s="211"/>
-      <c r="J42" s="211"/>
-      <c r="K42" s="211"/>
-      <c r="L42" s="192"/>
-      <c r="M42" s="192"/>
+      <c r="E42" s="249"/>
+      <c r="F42" s="252"/>
+      <c r="G42" s="251"/>
+      <c r="H42" s="250"/>
+      <c r="I42" s="250"/>
+      <c r="J42" s="250"/>
+      <c r="K42" s="250"/>
+      <c r="L42" s="261"/>
+      <c r="M42" s="261"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A43" s="226">
+      <c r="A43" s="223">
         <v>17</v>
       </c>
-      <c r="B43" s="257" t="s">
+      <c r="B43" s="213" t="s">
         <v>76</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>77</v>
       </c>
       <c r="D43" s="3"/>
-      <c r="E43" s="220" t="s">
+      <c r="E43" s="205" t="s">
         <v>70</v>
       </c>
-      <c r="F43" s="221"/>
-      <c r="G43" s="221"/>
-      <c r="H43" s="221"/>
-      <c r="I43" s="221"/>
-      <c r="J43" s="221"/>
-      <c r="K43" s="221"/>
-      <c r="L43" s="193"/>
-      <c r="M43" s="193"/>
+      <c r="F43" s="198"/>
+      <c r="G43" s="198"/>
+      <c r="H43" s="198"/>
+      <c r="I43" s="198"/>
+      <c r="J43" s="198"/>
+      <c r="K43" s="198"/>
+      <c r="L43" s="259"/>
+      <c r="M43" s="259"/>
     </row>
     <row r="44" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A44" s="227"/>
-      <c r="B44" s="258"/>
+      <c r="A44" s="211"/>
+      <c r="B44" s="214"/>
       <c r="C44" s="11" t="s">
         <v>80</v>
       </c>
       <c r="D44" s="4"/>
-      <c r="E44" s="215"/>
-      <c r="F44" s="212"/>
-      <c r="G44" s="212"/>
-      <c r="H44" s="212"/>
-      <c r="I44" s="212"/>
-      <c r="J44" s="212"/>
-      <c r="K44" s="212"/>
-      <c r="L44" s="190"/>
-      <c r="M44" s="190"/>
+      <c r="E44" s="200"/>
+      <c r="F44" s="194"/>
+      <c r="G44" s="194"/>
+      <c r="H44" s="194"/>
+      <c r="I44" s="194"/>
+      <c r="J44" s="194"/>
+      <c r="K44" s="194"/>
+      <c r="L44" s="242"/>
+      <c r="M44" s="242"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A45" s="235">
+      <c r="A45" s="210">
         <v>18</v>
       </c>
-      <c r="B45" s="258"/>
+      <c r="B45" s="214"/>
       <c r="C45" s="11" t="s">
         <v>81</v>
       </c>
       <c r="D45" s="4"/>
-      <c r="E45" s="207"/>
-      <c r="F45" s="214" t="s">
+      <c r="E45" s="193"/>
+      <c r="F45" s="203" t="s">
         <v>197</v>
       </c>
-      <c r="G45" s="210"/>
-      <c r="H45" s="214" t="s">
+      <c r="G45" s="197"/>
+      <c r="H45" s="203" t="s">
         <v>70</v>
       </c>
-      <c r="I45" s="214"/>
-      <c r="J45" s="214"/>
-      <c r="K45" s="214"/>
-      <c r="L45" s="194"/>
-      <c r="M45" s="194"/>
+      <c r="I45" s="203"/>
+      <c r="J45" s="203"/>
+      <c r="K45" s="203"/>
+      <c r="L45" s="253"/>
+      <c r="M45" s="253"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A46" s="235"/>
-      <c r="B46" s="258"/>
+      <c r="A46" s="210"/>
+      <c r="B46" s="214"/>
       <c r="C46" s="11" t="s">
         <v>83</v>
       </c>
       <c r="D46" s="4"/>
-      <c r="E46" s="207"/>
-      <c r="F46" s="214"/>
-      <c r="G46" s="210"/>
-      <c r="H46" s="214"/>
-      <c r="I46" s="214"/>
-      <c r="J46" s="214"/>
-      <c r="K46" s="214"/>
-      <c r="L46" s="194"/>
-      <c r="M46" s="194"/>
+      <c r="E46" s="193"/>
+      <c r="F46" s="203"/>
+      <c r="G46" s="197"/>
+      <c r="H46" s="203"/>
+      <c r="I46" s="203"/>
+      <c r="J46" s="203"/>
+      <c r="K46" s="203"/>
+      <c r="L46" s="253"/>
+      <c r="M46" s="253"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A47" s="227">
+      <c r="A47" s="211">
         <v>19</v>
       </c>
-      <c r="B47" s="258"/>
-      <c r="C47" s="260" t="s">
+      <c r="B47" s="214"/>
+      <c r="C47" s="216" t="s">
         <v>84</v>
       </c>
       <c r="D47" s="4"/>
-      <c r="E47" s="215" t="s">
+      <c r="E47" s="200" t="s">
         <v>78</v>
       </c>
-      <c r="F47" s="212"/>
-      <c r="G47" s="212"/>
-      <c r="H47" s="212"/>
-      <c r="I47" s="212"/>
-      <c r="J47" s="212"/>
-      <c r="K47" s="212"/>
-      <c r="L47" s="190"/>
-      <c r="M47" s="190"/>
+      <c r="F47" s="194"/>
+      <c r="G47" s="194"/>
+      <c r="H47" s="194"/>
+      <c r="I47" s="194"/>
+      <c r="J47" s="194"/>
+      <c r="K47" s="194"/>
+      <c r="L47" s="242"/>
+      <c r="M47" s="242"/>
     </row>
     <row r="48" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A48" s="228"/>
-      <c r="B48" s="259"/>
-      <c r="C48" s="261"/>
+      <c r="A48" s="212"/>
+      <c r="B48" s="215"/>
+      <c r="C48" s="217"/>
       <c r="D48" s="5"/>
-      <c r="E48" s="216"/>
-      <c r="F48" s="213"/>
-      <c r="G48" s="213"/>
-      <c r="H48" s="213"/>
-      <c r="I48" s="213"/>
-      <c r="J48" s="213"/>
-      <c r="K48" s="213"/>
-      <c r="L48" s="195"/>
-      <c r="M48" s="195"/>
+      <c r="E48" s="248"/>
+      <c r="F48" s="241"/>
+      <c r="G48" s="241"/>
+      <c r="H48" s="241"/>
+      <c r="I48" s="241"/>
+      <c r="J48" s="241"/>
+      <c r="K48" s="241"/>
+      <c r="L48" s="243"/>
+      <c r="M48" s="243"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A49" s="256">
+      <c r="A49" s="221">
         <v>20</v>
       </c>
-      <c r="B49" s="229" t="s">
+      <c r="B49" s="218" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>86</v>
       </c>
       <c r="D49" s="6"/>
-      <c r="E49" s="206"/>
-      <c r="F49" s="209"/>
-      <c r="G49" s="209"/>
-      <c r="H49" s="209" t="s">
+      <c r="E49" s="262"/>
+      <c r="F49" s="263"/>
+      <c r="G49" s="263"/>
+      <c r="H49" s="263" t="s">
         <v>78</v>
       </c>
-      <c r="I49" s="209"/>
-      <c r="J49" s="209"/>
-      <c r="K49" s="209"/>
-      <c r="L49" s="196"/>
-      <c r="M49" s="196"/>
+      <c r="I49" s="263"/>
+      <c r="J49" s="263"/>
+      <c r="K49" s="263"/>
+      <c r="L49" s="264"/>
+      <c r="M49" s="264"/>
     </row>
     <row r="50" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A50" s="235"/>
-      <c r="B50" s="230"/>
+      <c r="A50" s="210"/>
+      <c r="B50" s="219"/>
       <c r="C50" s="11" t="s">
         <v>87</v>
       </c>
       <c r="D50" s="4"/>
-      <c r="E50" s="207"/>
-      <c r="F50" s="210"/>
-      <c r="G50" s="210"/>
-      <c r="H50" s="210"/>
-      <c r="I50" s="210"/>
-      <c r="J50" s="210"/>
-      <c r="K50" s="210"/>
-      <c r="L50" s="191"/>
-      <c r="M50" s="191"/>
+      <c r="E50" s="193"/>
+      <c r="F50" s="197"/>
+      <c r="G50" s="197"/>
+      <c r="H50" s="197"/>
+      <c r="I50" s="197"/>
+      <c r="J50" s="197"/>
+      <c r="K50" s="197"/>
+      <c r="L50" s="260"/>
+      <c r="M50" s="260"/>
     </row>
     <row r="51" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A51" s="235"/>
-      <c r="B51" s="230"/>
+      <c r="A51" s="210"/>
+      <c r="B51" s="219"/>
       <c r="C51" s="11" t="s">
         <v>88</v>
       </c>
       <c r="D51" s="4"/>
-      <c r="E51" s="207"/>
-      <c r="F51" s="210"/>
-      <c r="G51" s="210"/>
-      <c r="H51" s="210"/>
-      <c r="I51" s="210"/>
-      <c r="J51" s="210"/>
-      <c r="K51" s="210"/>
-      <c r="L51" s="191"/>
-      <c r="M51" s="191"/>
+      <c r="E51" s="193"/>
+      <c r="F51" s="197"/>
+      <c r="G51" s="197"/>
+      <c r="H51" s="197"/>
+      <c r="I51" s="197"/>
+      <c r="J51" s="197"/>
+      <c r="K51" s="197"/>
+      <c r="L51" s="260"/>
+      <c r="M51" s="260"/>
     </row>
     <row r="52" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A52" s="262"/>
-      <c r="B52" s="231"/>
+      <c r="A52" s="222"/>
+      <c r="B52" s="220"/>
       <c r="C52" s="18" t="s">
         <v>89</v>
       </c>
       <c r="D52" s="5"/>
-      <c r="E52" s="208"/>
-      <c r="F52" s="211"/>
-      <c r="G52" s="211"/>
-      <c r="H52" s="211"/>
-      <c r="I52" s="211"/>
-      <c r="J52" s="211"/>
-      <c r="K52" s="211"/>
-      <c r="L52" s="192"/>
-      <c r="M52" s="192"/>
+      <c r="E52" s="249"/>
+      <c r="F52" s="250"/>
+      <c r="G52" s="250"/>
+      <c r="H52" s="250"/>
+      <c r="I52" s="250"/>
+      <c r="J52" s="250"/>
+      <c r="K52" s="250"/>
+      <c r="L52" s="261"/>
+      <c r="M52" s="261"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="56" spans="1:13" ht="15.75" thickBot="1">
@@ -14329,49 +14451,150 @@
     </row>
   </sheetData>
   <mergeCells count="211">
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="J2:J8"/>
-    <mergeCell ref="K2:K8"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="E2:E8"/>
-    <mergeCell ref="F2:F8"/>
-    <mergeCell ref="G2:G8"/>
-    <mergeCell ref="H2:H8"/>
-    <mergeCell ref="I2:I8"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B43:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B34:B42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B26:B33"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="M40:M42"/>
+    <mergeCell ref="M43:M44"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="M47:M48"/>
+    <mergeCell ref="M49:M52"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="M17:M19"/>
+    <mergeCell ref="M20:M22"/>
+    <mergeCell ref="M23:M25"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="M32:M33"/>
+    <mergeCell ref="M34:M35"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="M2:M8"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="L17:L19"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="L2:L8"/>
+    <mergeCell ref="E49:E52"/>
+    <mergeCell ref="F49:F52"/>
+    <mergeCell ref="G49:G52"/>
+    <mergeCell ref="H49:H52"/>
+    <mergeCell ref="I49:I52"/>
+    <mergeCell ref="J49:J52"/>
+    <mergeCell ref="K49:K52"/>
+    <mergeCell ref="L49:L52"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="I47:I48"/>
+    <mergeCell ref="J47:J48"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="I45:I46"/>
+    <mergeCell ref="J45:J46"/>
+    <mergeCell ref="K45:K46"/>
+    <mergeCell ref="L45:L46"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="K47:K48"/>
+    <mergeCell ref="L47:L48"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="H40:H42"/>
+    <mergeCell ref="I40:I42"/>
+    <mergeCell ref="J40:J42"/>
+    <mergeCell ref="K40:K42"/>
+    <mergeCell ref="L40:L42"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="K43:K44"/>
+    <mergeCell ref="L43:L44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="I43:I44"/>
+    <mergeCell ref="J43:J44"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="K38:K39"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="K34:K35"/>
+    <mergeCell ref="L34:L35"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="K36:K37"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="L32:L33"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="L23:L25"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="I20:I22"/>
+    <mergeCell ref="J20:J22"/>
+    <mergeCell ref="K20:K22"/>
+    <mergeCell ref="L20:L22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="I17:I19"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="K17:K19"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="I23:I25"/>
+    <mergeCell ref="J23:J25"/>
+    <mergeCell ref="K23:K25"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="B2:B8"/>
     <mergeCell ref="B9:B16"/>
@@ -14396,150 +14619,49 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="E17:E19"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="I17:I19"/>
-    <mergeCell ref="J17:J19"/>
-    <mergeCell ref="K17:K19"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="I23:I25"/>
-    <mergeCell ref="J23:J25"/>
-    <mergeCell ref="K23:K25"/>
-    <mergeCell ref="L23:L25"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="I20:I22"/>
-    <mergeCell ref="J20:J22"/>
-    <mergeCell ref="K20:K22"/>
-    <mergeCell ref="L20:L22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="L30:L31"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="L28:L29"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="L32:L33"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="J34:J35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="K38:K39"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="K34:K35"/>
-    <mergeCell ref="L34:L35"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="H36:H37"/>
-    <mergeCell ref="I36:I37"/>
-    <mergeCell ref="J36:J37"/>
-    <mergeCell ref="K36:K37"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="G40:G42"/>
-    <mergeCell ref="H40:H42"/>
-    <mergeCell ref="I40:I42"/>
-    <mergeCell ref="J40:J42"/>
-    <mergeCell ref="K40:K42"/>
-    <mergeCell ref="L40:L42"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="K43:K44"/>
-    <mergeCell ref="L43:L44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="I43:I44"/>
-    <mergeCell ref="J43:J44"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="I45:I46"/>
-    <mergeCell ref="J45:J46"/>
-    <mergeCell ref="K45:K46"/>
-    <mergeCell ref="L45:L46"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="K47:K48"/>
-    <mergeCell ref="L47:L48"/>
-    <mergeCell ref="E49:E52"/>
-    <mergeCell ref="F49:F52"/>
-    <mergeCell ref="G49:G52"/>
-    <mergeCell ref="H49:H52"/>
-    <mergeCell ref="I49:I52"/>
-    <mergeCell ref="J49:J52"/>
-    <mergeCell ref="K49:K52"/>
-    <mergeCell ref="L49:L52"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="I47:I48"/>
-    <mergeCell ref="J47:J48"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="M40:M42"/>
-    <mergeCell ref="M43:M44"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="M47:M48"/>
-    <mergeCell ref="M49:M52"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="M17:M19"/>
-    <mergeCell ref="M20:M22"/>
-    <mergeCell ref="M23:M25"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="M28:M29"/>
-    <mergeCell ref="M30:M31"/>
-    <mergeCell ref="M32:M33"/>
-    <mergeCell ref="M34:M35"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="M2:M8"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="L17:L19"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="L2:L8"/>
+    <mergeCell ref="B26:B33"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B43:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B34:B42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="J2:J8"/>
+    <mergeCell ref="K2:K8"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="E2:E8"/>
+    <mergeCell ref="F2:F8"/>
+    <mergeCell ref="G2:G8"/>
+    <mergeCell ref="H2:H8"/>
+    <mergeCell ref="I2:I8"/>
+    <mergeCell ref="I11:I12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="https://drive.google.com/open?id=1RYgFxmL-dmZYtjF2ca5a0yQUWnMVjo3mVexJabJL1c4"/>
@@ -14655,8 +14777,8 @@
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -14700,10 +14822,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A2" s="282" t="s">
+      <c r="A2" s="278" t="s">
         <v>305</v>
       </c>
-      <c r="B2" s="277">
+      <c r="B2" s="271">
         <v>1</v>
       </c>
       <c r="C2" s="110">
@@ -14723,8 +14845,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A3" s="283"/>
-      <c r="B3" s="278"/>
+      <c r="A3" s="279"/>
+      <c r="B3" s="272"/>
       <c r="C3" s="110">
         <v>43193</v>
       </c>
@@ -14740,8 +14862,8 @@
       <c r="I3" s="115"/>
     </row>
     <row r="4" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A4" s="283"/>
-      <c r="B4" s="278"/>
+      <c r="A4" s="279"/>
+      <c r="B4" s="272"/>
       <c r="C4" s="110">
         <v>43194</v>
       </c>
@@ -14757,8 +14879,8 @@
       <c r="I4" s="115"/>
     </row>
     <row r="5" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A5" s="283"/>
-      <c r="B5" s="278"/>
+      <c r="A5" s="279"/>
+      <c r="B5" s="272"/>
       <c r="C5" s="110">
         <v>43195</v>
       </c>
@@ -14776,8 +14898,8 @@
       <c r="I5" s="115"/>
     </row>
     <row r="6" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A6" s="284"/>
-      <c r="B6" s="281"/>
+      <c r="A6" s="280"/>
+      <c r="B6" s="273"/>
       <c r="C6" s="117">
         <v>43196</v>
       </c>
@@ -14793,10 +14915,10 @@
       <c r="I6" s="121"/>
     </row>
     <row r="7" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A7" s="292" t="s">
+      <c r="A7" s="285" t="s">
         <v>184</v>
       </c>
-      <c r="B7" s="280">
+      <c r="B7" s="281">
         <v>2</v>
       </c>
       <c r="C7" s="143">
@@ -14814,8 +14936,8 @@
       <c r="I7" s="126"/>
     </row>
     <row r="8" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A8" s="293"/>
-      <c r="B8" s="275"/>
+      <c r="A8" s="286"/>
+      <c r="B8" s="282"/>
       <c r="C8" s="143">
         <v>43200</v>
       </c>
@@ -14831,8 +14953,8 @@
       <c r="I8" s="126"/>
     </row>
     <row r="9" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A9" s="293"/>
-      <c r="B9" s="275"/>
+      <c r="A9" s="286"/>
+      <c r="B9" s="282"/>
       <c r="C9" s="143">
         <v>43201</v>
       </c>
@@ -14848,8 +14970,8 @@
       <c r="I9" s="126"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A10" s="293"/>
-      <c r="B10" s="275"/>
+      <c r="A10" s="286"/>
+      <c r="B10" s="282"/>
       <c r="C10" s="143">
         <v>43202</v>
       </c>
@@ -14865,8 +14987,8 @@
       <c r="I10" s="126"/>
     </row>
     <row r="11" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A11" s="293"/>
-      <c r="B11" s="285"/>
+      <c r="A11" s="286"/>
+      <c r="B11" s="283"/>
       <c r="C11" s="143">
         <v>43203</v>
       </c>
@@ -14884,8 +15006,8 @@
       <c r="I11" s="126"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A12" s="272"/>
-      <c r="B12" s="286">
+      <c r="A12" s="287"/>
+      <c r="B12" s="277">
         <v>3</v>
       </c>
       <c r="C12" s="110">
@@ -14903,8 +15025,8 @@
       <c r="I12" s="115"/>
     </row>
     <row r="13" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A13" s="272"/>
-      <c r="B13" s="278"/>
+      <c r="A13" s="287"/>
+      <c r="B13" s="272"/>
       <c r="C13" s="110">
         <v>43207</v>
       </c>
@@ -14920,8 +15042,8 @@
       <c r="I13" s="115"/>
     </row>
     <row r="14" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A14" s="272"/>
-      <c r="B14" s="278"/>
+      <c r="A14" s="287"/>
+      <c r="B14" s="272"/>
       <c r="C14" s="110">
         <v>43208</v>
       </c>
@@ -14937,8 +15059,8 @@
       <c r="I14" s="115"/>
     </row>
     <row r="15" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A15" s="272"/>
-      <c r="B15" s="278"/>
+      <c r="A15" s="287"/>
+      <c r="B15" s="272"/>
       <c r="C15" s="110">
         <v>43209</v>
       </c>
@@ -14954,8 +15076,8 @@
       <c r="I15" s="115"/>
     </row>
     <row r="16" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A16" s="272"/>
-      <c r="B16" s="279"/>
+      <c r="A16" s="287"/>
+      <c r="B16" s="284"/>
       <c r="C16" s="110">
         <v>43210</v>
       </c>
@@ -14971,8 +15093,8 @@
       <c r="I16" s="115"/>
     </row>
     <row r="17" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A17" s="272"/>
-      <c r="B17" s="280">
+      <c r="A17" s="287"/>
+      <c r="B17" s="281">
         <v>4</v>
       </c>
       <c r="C17" s="122">
@@ -14994,8 +15116,8 @@
       <c r="I17" s="126"/>
     </row>
     <row r="18" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A18" s="272"/>
-      <c r="B18" s="275"/>
+      <c r="A18" s="287"/>
+      <c r="B18" s="282"/>
       <c r="C18" s="122">
         <v>43214</v>
       </c>
@@ -15011,8 +15133,8 @@
       <c r="I18" s="126"/>
     </row>
     <row r="19" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A19" s="272"/>
-      <c r="B19" s="275"/>
+      <c r="A19" s="287"/>
+      <c r="B19" s="282"/>
       <c r="C19" s="122">
         <v>43215</v>
       </c>
@@ -15028,8 +15150,8 @@
       <c r="I19" s="126"/>
     </row>
     <row r="20" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A20" s="272"/>
-      <c r="B20" s="275"/>
+      <c r="A20" s="287"/>
+      <c r="B20" s="282"/>
       <c r="C20" s="122">
         <v>43216</v>
       </c>
@@ -15045,8 +15167,8 @@
       <c r="I20" s="126"/>
     </row>
     <row r="21" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A21" s="272"/>
-      <c r="B21" s="285"/>
+      <c r="A21" s="287"/>
+      <c r="B21" s="283"/>
       <c r="C21" s="122">
         <v>43217</v>
       </c>
@@ -15064,8 +15186,8 @@
       <c r="I21" s="126"/>
     </row>
     <row r="22" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A22" s="272"/>
-      <c r="B22" s="286">
+      <c r="A22" s="287"/>
+      <c r="B22" s="277">
         <v>5</v>
       </c>
       <c r="C22" s="110">
@@ -15083,8 +15205,8 @@
       <c r="I22" s="115"/>
     </row>
     <row r="23" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A23" s="272"/>
-      <c r="B23" s="278"/>
+      <c r="A23" s="287"/>
+      <c r="B23" s="272"/>
       <c r="C23" s="110">
         <v>43221</v>
       </c>
@@ -15100,8 +15222,8 @@
       <c r="I23" s="115"/>
     </row>
     <row r="24" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A24" s="272"/>
-      <c r="B24" s="278"/>
+      <c r="A24" s="287"/>
+      <c r="B24" s="272"/>
       <c r="C24" s="110">
         <v>43222</v>
       </c>
@@ -15117,8 +15239,8 @@
       <c r="I24" s="115"/>
     </row>
     <row r="25" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A25" s="272"/>
-      <c r="B25" s="278"/>
+      <c r="A25" s="287"/>
+      <c r="B25" s="272"/>
       <c r="C25" s="110">
         <v>43223</v>
       </c>
@@ -15134,8 +15256,8 @@
       <c r="I25" s="115"/>
     </row>
     <row r="26" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A26" s="272"/>
-      <c r="B26" s="279"/>
+      <c r="A26" s="287"/>
+      <c r="B26" s="284"/>
       <c r="C26" s="110">
         <v>43224</v>
       </c>
@@ -15151,8 +15273,8 @@
       <c r="I26" s="115"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A27" s="272"/>
-      <c r="B27" s="290">
+      <c r="A27" s="287"/>
+      <c r="B27" s="289">
         <v>6</v>
       </c>
       <c r="C27" s="130">
@@ -15174,8 +15296,8 @@
       <c r="I27" s="126"/>
     </row>
     <row r="28" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A28" s="272"/>
-      <c r="B28" s="288"/>
+      <c r="A28" s="287"/>
+      <c r="B28" s="275"/>
       <c r="C28" s="130">
         <v>43228</v>
       </c>
@@ -15191,8 +15313,8 @@
       <c r="I28" s="126"/>
     </row>
     <row r="29" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A29" s="272"/>
-      <c r="B29" s="288"/>
+      <c r="A29" s="287"/>
+      <c r="B29" s="275"/>
       <c r="C29" s="130">
         <v>43229</v>
       </c>
@@ -15208,8 +15330,8 @@
       <c r="I29" s="126"/>
     </row>
     <row r="30" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A30" s="272"/>
-      <c r="B30" s="288"/>
+      <c r="A30" s="287"/>
+      <c r="B30" s="275"/>
       <c r="C30" s="130">
         <v>43230</v>
       </c>
@@ -15225,8 +15347,8 @@
       <c r="I30" s="126"/>
     </row>
     <row r="31" spans="1:9" ht="27" thickBot="1">
-      <c r="A31" s="273"/>
-      <c r="B31" s="291"/>
+      <c r="A31" s="288"/>
+      <c r="B31" s="290"/>
       <c r="C31" s="134">
         <v>43231</v>
       </c>
@@ -15244,10 +15366,10 @@
       <c r="I31" s="138"/>
     </row>
     <row r="32" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A32" s="282" t="s">
+      <c r="A32" s="278" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="277">
+      <c r="B32" s="271">
         <v>7</v>
       </c>
       <c r="C32" s="110">
@@ -15265,8 +15387,8 @@
       <c r="I32" s="115"/>
     </row>
     <row r="33" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A33" s="283"/>
-      <c r="B33" s="278"/>
+      <c r="A33" s="279"/>
+      <c r="B33" s="272"/>
       <c r="C33" s="110">
         <v>43235</v>
       </c>
@@ -15282,8 +15404,8 @@
       <c r="I33" s="115"/>
     </row>
     <row r="34" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A34" s="283"/>
-      <c r="B34" s="278"/>
+      <c r="A34" s="279"/>
+      <c r="B34" s="272"/>
       <c r="C34" s="110">
         <v>43236</v>
       </c>
@@ -15299,8 +15421,8 @@
       <c r="I34" s="115"/>
     </row>
     <row r="35" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A35" s="283"/>
-      <c r="B35" s="278"/>
+      <c r="A35" s="279"/>
+      <c r="B35" s="272"/>
       <c r="C35" s="110">
         <v>43237</v>
       </c>
@@ -15316,8 +15438,8 @@
       <c r="I35" s="115"/>
     </row>
     <row r="36" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A36" s="283"/>
-      <c r="B36" s="281"/>
+      <c r="A36" s="279"/>
+      <c r="B36" s="273"/>
       <c r="C36" s="110">
         <v>43238</v>
       </c>
@@ -15333,8 +15455,8 @@
       <c r="I36" s="115"/>
     </row>
     <row r="37" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A37" s="283"/>
-      <c r="B37" s="287">
+      <c r="A37" s="279"/>
+      <c r="B37" s="274">
         <v>8</v>
       </c>
       <c r="C37" s="130">
@@ -15356,8 +15478,8 @@
       <c r="I37" s="126"/>
     </row>
     <row r="38" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A38" s="283"/>
-      <c r="B38" s="288"/>
+      <c r="A38" s="279"/>
+      <c r="B38" s="275"/>
       <c r="C38" s="130">
         <v>43242</v>
       </c>
@@ -15373,8 +15495,8 @@
       <c r="I38" s="126"/>
     </row>
     <row r="39" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A39" s="283"/>
-      <c r="B39" s="288"/>
+      <c r="A39" s="279"/>
+      <c r="B39" s="275"/>
       <c r="C39" s="130">
         <v>43243</v>
       </c>
@@ -15390,8 +15512,8 @@
       <c r="I39" s="126"/>
     </row>
     <row r="40" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A40" s="283"/>
-      <c r="B40" s="288"/>
+      <c r="A40" s="279"/>
+      <c r="B40" s="275"/>
       <c r="C40" s="130">
         <v>43244</v>
       </c>
@@ -15407,8 +15529,8 @@
       <c r="I40" s="126"/>
     </row>
     <row r="41" spans="1:9" ht="27" thickBot="1">
-      <c r="A41" s="283"/>
-      <c r="B41" s="289"/>
+      <c r="A41" s="279"/>
+      <c r="B41" s="276"/>
       <c r="C41" s="130">
         <v>43245</v>
       </c>
@@ -15426,8 +15548,8 @@
       <c r="I41" s="126"/>
     </row>
     <row r="42" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A42" s="283"/>
-      <c r="B42" s="286">
+      <c r="A42" s="279"/>
+      <c r="B42" s="277">
         <v>9</v>
       </c>
       <c r="C42" s="110">
@@ -15445,8 +15567,8 @@
       <c r="I42" s="115"/>
     </row>
     <row r="43" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A43" s="283"/>
-      <c r="B43" s="278"/>
+      <c r="A43" s="279"/>
+      <c r="B43" s="272"/>
       <c r="C43" s="110">
         <v>43249</v>
       </c>
@@ -15462,8 +15584,8 @@
       <c r="I43" s="115"/>
     </row>
     <row r="44" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A44" s="283"/>
-      <c r="B44" s="278"/>
+      <c r="A44" s="279"/>
+      <c r="B44" s="272"/>
       <c r="C44" s="110">
         <v>43250</v>
       </c>
@@ -15479,8 +15601,8 @@
       <c r="I44" s="115"/>
     </row>
     <row r="45" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A45" s="283"/>
-      <c r="B45" s="278"/>
+      <c r="A45" s="279"/>
+      <c r="B45" s="272"/>
       <c r="C45" s="110">
         <v>43251</v>
       </c>
@@ -15496,8 +15618,8 @@
       <c r="I45" s="115"/>
     </row>
     <row r="46" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A46" s="284"/>
-      <c r="B46" s="281"/>
+      <c r="A46" s="280"/>
+      <c r="B46" s="273"/>
       <c r="C46" s="117">
         <v>43252</v>
       </c>
@@ -15513,10 +15635,10 @@
       <c r="I46" s="121"/>
     </row>
     <row r="47" spans="1:9" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A47" s="271" t="s">
+      <c r="A47" s="293" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="274">
+      <c r="B47" s="291">
         <v>10</v>
       </c>
       <c r="C47" s="122">
@@ -15538,8 +15660,8 @@
       <c r="I47" s="126"/>
     </row>
     <row r="48" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A48" s="272"/>
-      <c r="B48" s="275"/>
+      <c r="A48" s="287"/>
+      <c r="B48" s="282"/>
       <c r="C48" s="122">
         <v>43256</v>
       </c>
@@ -15555,8 +15677,8 @@
       <c r="I48" s="126"/>
     </row>
     <row r="49" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A49" s="272"/>
-      <c r="B49" s="275"/>
+      <c r="A49" s="287"/>
+      <c r="B49" s="282"/>
       <c r="C49" s="122">
         <v>43257</v>
       </c>
@@ -15572,8 +15694,8 @@
       <c r="I49" s="126"/>
     </row>
     <row r="50" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A50" s="272"/>
-      <c r="B50" s="275"/>
+      <c r="A50" s="287"/>
+      <c r="B50" s="282"/>
       <c r="C50" s="122">
         <v>43258</v>
       </c>
@@ -15589,8 +15711,8 @@
       <c r="I50" s="126"/>
     </row>
     <row r="51" spans="1:9" ht="27" thickBot="1">
-      <c r="A51" s="272"/>
-      <c r="B51" s="276"/>
+      <c r="A51" s="287"/>
+      <c r="B51" s="292"/>
       <c r="C51" s="122">
         <v>43259</v>
       </c>
@@ -15608,8 +15730,8 @@
       <c r="I51" s="126"/>
     </row>
     <row r="52" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A52" s="272"/>
-      <c r="B52" s="277">
+      <c r="A52" s="287"/>
+      <c r="B52" s="271">
         <v>11</v>
       </c>
       <c r="C52" s="110">
@@ -15627,8 +15749,8 @@
       <c r="I52" s="115"/>
     </row>
     <row r="53" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A53" s="272"/>
-      <c r="B53" s="278"/>
+      <c r="A53" s="287"/>
+      <c r="B53" s="272"/>
       <c r="C53" s="110">
         <v>43263</v>
       </c>
@@ -15644,8 +15766,8 @@
       <c r="I53" s="115"/>
     </row>
     <row r="54" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A54" s="272"/>
-      <c r="B54" s="278"/>
+      <c r="A54" s="287"/>
+      <c r="B54" s="272"/>
       <c r="C54" s="110">
         <v>43264</v>
       </c>
@@ -15661,8 +15783,8 @@
       <c r="I54" s="115"/>
     </row>
     <row r="55" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A55" s="272"/>
-      <c r="B55" s="278"/>
+      <c r="A55" s="287"/>
+      <c r="B55" s="272"/>
       <c r="C55" s="110">
         <v>43265</v>
       </c>
@@ -15678,8 +15800,8 @@
       <c r="I55" s="115"/>
     </row>
     <row r="56" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A56" s="272"/>
-      <c r="B56" s="279"/>
+      <c r="A56" s="287"/>
+      <c r="B56" s="284"/>
       <c r="C56" s="110">
         <v>43266</v>
       </c>
@@ -15695,8 +15817,8 @@
       <c r="I56" s="115"/>
     </row>
     <row r="57" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A57" s="272"/>
-      <c r="B57" s="280">
+      <c r="A57" s="287"/>
+      <c r="B57" s="281">
         <v>12</v>
       </c>
       <c r="C57" s="122">
@@ -15718,8 +15840,8 @@
       <c r="I57" s="126"/>
     </row>
     <row r="58" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A58" s="272"/>
-      <c r="B58" s="275"/>
+      <c r="A58" s="287"/>
+      <c r="B58" s="282"/>
       <c r="C58" s="122">
         <v>43270</v>
       </c>
@@ -15735,8 +15857,8 @@
       <c r="I58" s="126"/>
     </row>
     <row r="59" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A59" s="272"/>
-      <c r="B59" s="275"/>
+      <c r="A59" s="287"/>
+      <c r="B59" s="282"/>
       <c r="C59" s="122">
         <v>43271</v>
       </c>
@@ -15752,8 +15874,8 @@
       <c r="I59" s="126"/>
     </row>
     <row r="60" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A60" s="272"/>
-      <c r="B60" s="275"/>
+      <c r="A60" s="287"/>
+      <c r="B60" s="282"/>
       <c r="C60" s="122">
         <v>43272</v>
       </c>
@@ -15769,8 +15891,8 @@
       <c r="I60" s="126"/>
     </row>
     <row r="61" spans="1:9" ht="27" thickBot="1">
-      <c r="A61" s="273"/>
-      <c r="B61" s="276"/>
+      <c r="A61" s="288"/>
+      <c r="B61" s="292"/>
       <c r="C61" s="140">
         <v>43273</v>
       </c>
@@ -15788,10 +15910,10 @@
       <c r="I61" s="138"/>
     </row>
     <row r="62" spans="1:9" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A62" s="282" t="s">
+      <c r="A62" s="278" t="s">
         <v>627</v>
       </c>
-      <c r="B62" s="277">
+      <c r="B62" s="271">
         <v>13</v>
       </c>
       <c r="C62" s="110">
@@ -15809,8 +15931,8 @@
       <c r="I62" s="115"/>
     </row>
     <row r="63" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A63" s="283"/>
-      <c r="B63" s="278"/>
+      <c r="A63" s="279"/>
+      <c r="B63" s="272"/>
       <c r="C63" s="110">
         <v>43277</v>
       </c>
@@ -15826,8 +15948,8 @@
       <c r="I63" s="115"/>
     </row>
     <row r="64" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A64" s="283"/>
-      <c r="B64" s="278"/>
+      <c r="A64" s="279"/>
+      <c r="B64" s="272"/>
       <c r="C64" s="110">
         <v>43278</v>
       </c>
@@ -15843,8 +15965,8 @@
       <c r="I64" s="115"/>
     </row>
     <row r="65" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A65" s="283"/>
-      <c r="B65" s="278"/>
+      <c r="A65" s="279"/>
+      <c r="B65" s="272"/>
       <c r="C65" s="110">
         <v>43279</v>
       </c>
@@ -15860,8 +15982,8 @@
       <c r="I65" s="115"/>
     </row>
     <row r="66" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A66" s="283"/>
-      <c r="B66" s="281"/>
+      <c r="A66" s="279"/>
+      <c r="B66" s="273"/>
       <c r="C66" s="110">
         <v>43280</v>
       </c>
@@ -15877,8 +15999,8 @@
       <c r="I66" s="115"/>
     </row>
     <row r="67" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A67" s="283"/>
-      <c r="B67" s="287">
+      <c r="A67" s="279"/>
+      <c r="B67" s="274">
         <v>14</v>
       </c>
       <c r="C67" s="130">
@@ -15900,8 +16022,8 @@
       <c r="I67" s="126"/>
     </row>
     <row r="68" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A68" s="283"/>
-      <c r="B68" s="288"/>
+      <c r="A68" s="279"/>
+      <c r="B68" s="275"/>
       <c r="C68" s="130">
         <v>43284</v>
       </c>
@@ -15917,8 +16039,8 @@
       <c r="I68" s="126"/>
     </row>
     <row r="69" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A69" s="283"/>
-      <c r="B69" s="288"/>
+      <c r="A69" s="279"/>
+      <c r="B69" s="275"/>
       <c r="C69" s="130">
         <v>43285</v>
       </c>
@@ -15934,8 +16056,8 @@
       <c r="I69" s="126"/>
     </row>
     <row r="70" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A70" s="283"/>
-      <c r="B70" s="288"/>
+      <c r="A70" s="279"/>
+      <c r="B70" s="275"/>
       <c r="C70" s="130">
         <v>43286</v>
       </c>
@@ -15951,8 +16073,8 @@
       <c r="I70" s="126"/>
     </row>
     <row r="71" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A71" s="283"/>
-      <c r="B71" s="289"/>
+      <c r="A71" s="279"/>
+      <c r="B71" s="276"/>
       <c r="C71" s="130">
         <v>43287</v>
       </c>
@@ -15970,8 +16092,8 @@
       <c r="I71" s="126"/>
     </row>
     <row r="72" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A72" s="283"/>
-      <c r="B72" s="286">
+      <c r="A72" s="279"/>
+      <c r="B72" s="277">
         <v>15</v>
       </c>
       <c r="C72" s="110">
@@ -15989,8 +16111,8 @@
       <c r="I72" s="115"/>
     </row>
     <row r="73" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A73" s="283"/>
-      <c r="B73" s="278"/>
+      <c r="A73" s="279"/>
+      <c r="B73" s="272"/>
       <c r="C73" s="110">
         <v>43291</v>
       </c>
@@ -16006,8 +16128,8 @@
       <c r="I73" s="115"/>
     </row>
     <row r="74" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A74" s="283"/>
-      <c r="B74" s="278"/>
+      <c r="A74" s="279"/>
+      <c r="B74" s="272"/>
       <c r="C74" s="110">
         <v>43292</v>
       </c>
@@ -16023,8 +16145,8 @@
       <c r="I74" s="115"/>
     </row>
     <row r="75" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A75" s="283"/>
-      <c r="B75" s="278"/>
+      <c r="A75" s="279"/>
+      <c r="B75" s="272"/>
       <c r="C75" s="110">
         <v>43293</v>
       </c>
@@ -16040,8 +16162,8 @@
       <c r="I75" s="115"/>
     </row>
     <row r="76" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A76" s="283"/>
-      <c r="B76" s="279"/>
+      <c r="A76" s="279"/>
+      <c r="B76" s="284"/>
       <c r="C76" s="110">
         <v>43294</v>
       </c>
@@ -16057,8 +16179,8 @@
       <c r="I76" s="115"/>
     </row>
     <row r="77" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A77" s="283"/>
-      <c r="B77" s="290">
+      <c r="A77" s="279"/>
+      <c r="B77" s="289">
         <v>16</v>
       </c>
       <c r="C77" s="130">
@@ -16080,8 +16202,8 @@
       <c r="I77" s="126"/>
     </row>
     <row r="78" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A78" s="283"/>
-      <c r="B78" s="288"/>
+      <c r="A78" s="279"/>
+      <c r="B78" s="275"/>
       <c r="C78" s="130">
         <v>43298</v>
       </c>
@@ -16097,8 +16219,8 @@
       <c r="I78" s="126"/>
     </row>
     <row r="79" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A79" s="283"/>
-      <c r="B79" s="288"/>
+      <c r="A79" s="279"/>
+      <c r="B79" s="275"/>
       <c r="C79" s="130">
         <v>43299</v>
       </c>
@@ -16114,8 +16236,8 @@
       <c r="I79" s="126"/>
     </row>
     <row r="80" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A80" s="283"/>
-      <c r="B80" s="288"/>
+      <c r="A80" s="279"/>
+      <c r="B80" s="275"/>
       <c r="C80" s="130">
         <v>43300</v>
       </c>
@@ -16131,8 +16253,8 @@
       <c r="I80" s="126"/>
     </row>
     <row r="81" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A81" s="284"/>
-      <c r="B81" s="291"/>
+      <c r="A81" s="280"/>
+      <c r="B81" s="290"/>
       <c r="C81" s="134">
         <v>43301</v>
       </c>
@@ -16150,10 +16272,10 @@
       <c r="I81" s="138"/>
     </row>
     <row r="82" spans="1:9" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A82" s="282" t="s">
+      <c r="A82" s="278" t="s">
         <v>76</v>
       </c>
-      <c r="B82" s="277">
+      <c r="B82" s="271">
         <v>17</v>
       </c>
       <c r="C82" s="110">
@@ -16171,8 +16293,8 @@
       <c r="I82" s="115"/>
     </row>
     <row r="83" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A83" s="283"/>
-      <c r="B83" s="278"/>
+      <c r="A83" s="279"/>
+      <c r="B83" s="272"/>
       <c r="C83" s="110">
         <v>43305</v>
       </c>
@@ -16188,8 +16310,8 @@
       <c r="I83" s="115"/>
     </row>
     <row r="84" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A84" s="283"/>
-      <c r="B84" s="278"/>
+      <c r="A84" s="279"/>
+      <c r="B84" s="272"/>
       <c r="C84" s="110">
         <v>43306</v>
       </c>
@@ -16205,8 +16327,8 @@
       <c r="I84" s="115"/>
     </row>
     <row r="85" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A85" s="283"/>
-      <c r="B85" s="278"/>
+      <c r="A85" s="279"/>
+      <c r="B85" s="272"/>
       <c r="C85" s="110">
         <v>43307</v>
       </c>
@@ -16222,8 +16344,8 @@
       <c r="I85" s="115"/>
     </row>
     <row r="86" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A86" s="284"/>
-      <c r="B86" s="281"/>
+      <c r="A86" s="280"/>
+      <c r="B86" s="273"/>
       <c r="C86" s="117">
         <v>43308</v>
       </c>
@@ -16239,10 +16361,10 @@
       <c r="I86" s="121"/>
     </row>
     <row r="87" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A87" s="282" t="s">
+      <c r="A87" s="278" t="s">
         <v>632</v>
       </c>
-      <c r="B87" s="274">
+      <c r="B87" s="291">
         <v>18</v>
       </c>
       <c r="C87" s="122">
@@ -16264,8 +16386,8 @@
       <c r="I87" s="126"/>
     </row>
     <row r="88" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A88" s="283"/>
-      <c r="B88" s="275"/>
+      <c r="A88" s="279"/>
+      <c r="B88" s="282"/>
       <c r="C88" s="122">
         <v>43312</v>
       </c>
@@ -16281,8 +16403,8 @@
       <c r="I88" s="126"/>
     </row>
     <row r="89" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A89" s="283"/>
-      <c r="B89" s="275"/>
+      <c r="A89" s="279"/>
+      <c r="B89" s="282"/>
       <c r="C89" s="122">
         <v>43313</v>
       </c>
@@ -16298,8 +16420,8 @@
       <c r="I89" s="126"/>
     </row>
     <row r="90" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A90" s="283"/>
-      <c r="B90" s="275"/>
+      <c r="A90" s="279"/>
+      <c r="B90" s="282"/>
       <c r="C90" s="122">
         <v>43314</v>
       </c>
@@ -16315,8 +16437,8 @@
       <c r="I90" s="126"/>
     </row>
     <row r="91" spans="1:9" ht="27" thickBot="1">
-      <c r="A91" s="283"/>
-      <c r="B91" s="285"/>
+      <c r="A91" s="279"/>
+      <c r="B91" s="283"/>
       <c r="C91" s="122">
         <v>43315</v>
       </c>
@@ -16334,8 +16456,8 @@
       <c r="I91" s="126"/>
     </row>
     <row r="92" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A92" s="283"/>
-      <c r="B92" s="286">
+      <c r="A92" s="279"/>
+      <c r="B92" s="277">
         <v>19</v>
       </c>
       <c r="C92" s="110">
@@ -16353,8 +16475,8 @@
       <c r="I92" s="115"/>
     </row>
     <row r="93" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A93" s="283"/>
-      <c r="B93" s="278"/>
+      <c r="A93" s="279"/>
+      <c r="B93" s="272"/>
       <c r="C93" s="110">
         <v>43319</v>
       </c>
@@ -16370,8 +16492,8 @@
       <c r="I93" s="115"/>
     </row>
     <row r="94" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A94" s="283"/>
-      <c r="B94" s="278"/>
+      <c r="A94" s="279"/>
+      <c r="B94" s="272"/>
       <c r="C94" s="110">
         <v>43320</v>
       </c>
@@ -16387,8 +16509,8 @@
       <c r="I94" s="115"/>
     </row>
     <row r="95" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A95" s="283"/>
-      <c r="B95" s="278"/>
+      <c r="A95" s="279"/>
+      <c r="B95" s="272"/>
       <c r="C95" s="110">
         <v>43321</v>
       </c>
@@ -16404,8 +16526,8 @@
       <c r="I95" s="115"/>
     </row>
     <row r="96" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A96" s="283"/>
-      <c r="B96" s="279"/>
+      <c r="A96" s="279"/>
+      <c r="B96" s="284"/>
       <c r="C96" s="110">
         <v>43322</v>
       </c>
@@ -16421,8 +16543,8 @@
       <c r="I96" s="115"/>
     </row>
     <row r="97" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A97" s="283"/>
-      <c r="B97" s="280">
+      <c r="A97" s="279"/>
+      <c r="B97" s="281">
         <v>20</v>
       </c>
       <c r="C97" s="122">
@@ -16442,8 +16564,8 @@
       <c r="I97" s="126"/>
     </row>
     <row r="98" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A98" s="283"/>
-      <c r="B98" s="275"/>
+      <c r="A98" s="279"/>
+      <c r="B98" s="282"/>
       <c r="C98" s="122">
         <v>43326</v>
       </c>
@@ -16459,8 +16581,8 @@
       <c r="I98" s="126"/>
     </row>
     <row r="99" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A99" s="283"/>
-      <c r="B99" s="275"/>
+      <c r="A99" s="279"/>
+      <c r="B99" s="282"/>
       <c r="C99" s="122">
         <v>43327</v>
       </c>
@@ -16476,8 +16598,8 @@
       <c r="I99" s="126"/>
     </row>
     <row r="100" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A100" s="283"/>
-      <c r="B100" s="275"/>
+      <c r="A100" s="279"/>
+      <c r="B100" s="282"/>
       <c r="C100" s="122">
         <v>43328</v>
       </c>
@@ -16495,8 +16617,8 @@
       <c r="I100" s="126"/>
     </row>
     <row r="101" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A101" s="284"/>
-      <c r="B101" s="276"/>
+      <c r="A101" s="280"/>
+      <c r="B101" s="292"/>
       <c r="C101" s="140">
         <v>43329</v>
       </c>
@@ -22806,6 +22928,21 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A47:A61"/>
+    <mergeCell ref="B47:B51"/>
+    <mergeCell ref="B52:B56"/>
+    <mergeCell ref="B57:B61"/>
+    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="A87:A101"/>
+    <mergeCell ref="A62:A81"/>
+    <mergeCell ref="B87:B91"/>
+    <mergeCell ref="B92:B96"/>
+    <mergeCell ref="B97:B101"/>
+    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="B72:B76"/>
+    <mergeCell ref="B77:B81"/>
+    <mergeCell ref="B82:B86"/>
     <mergeCell ref="B32:B36"/>
     <mergeCell ref="B37:B41"/>
     <mergeCell ref="B42:B46"/>
@@ -22818,21 +22955,6 @@
     <mergeCell ref="B22:B26"/>
     <mergeCell ref="B27:B31"/>
     <mergeCell ref="A32:A46"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="A87:A101"/>
-    <mergeCell ref="A62:A81"/>
-    <mergeCell ref="B87:B91"/>
-    <mergeCell ref="B92:B96"/>
-    <mergeCell ref="B97:B101"/>
-    <mergeCell ref="B67:B71"/>
-    <mergeCell ref="B72:B76"/>
-    <mergeCell ref="B77:B81"/>
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="A47:A61"/>
-    <mergeCell ref="B47:B51"/>
-    <mergeCell ref="B52:B56"/>
-    <mergeCell ref="B57:B61"/>
-    <mergeCell ref="B62:B66"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://drive.google.com/open?id=12f1t9Kg0CD9OW5iG5jB3Ozx_iRGw-cbyozVUPhhG6ME"/>
@@ -22847,8 +22969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -28979,10 +29101,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -29025,6 +29147,56 @@
     <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>970</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="24" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="301" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="300" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="302" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="302" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="302" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="300" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="300" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="300" t="s">
+        <v>999</v>
       </c>
     </row>
   </sheetData>
@@ -29035,10 +29207,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:A53"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -29249,11 +29421,17 @@
         <v>887</v>
       </c>
     </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="22" t="s">
+        <v>963</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A20" r:id="rId1" location="js" display="https://code.sololearn.com/658/ - js"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Thursday May 31 Afternoon
</commit_message>
<xml_diff>
--- a/General/Curriculum (Personalized).xlsx
+++ b/General/Curriculum (Personalized).xlsx
@@ -12036,115 +12036,76 @@
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="37" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12152,6 +12113,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -12162,55 +12138,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12231,71 +12177,116 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="37" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -12303,13 +12294,19 @@
     <xf numFmtId="0" fontId="14" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12321,20 +12318,29 @@
     <xf numFmtId="0" fontId="35" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -12342,10 +12348,13 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
@@ -12365,15 +12374,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -13393,21 +13393,21 @@
       <c r="H1" s="35" t="s">
         <v>193</v>
       </c>
-      <c r="I1" s="263" t="s">
+      <c r="I1" s="193" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="264"/>
-      <c r="K1" s="265"/>
-      <c r="L1" s="197" t="s">
+      <c r="J1" s="194"/>
+      <c r="K1" s="195"/>
+      <c r="L1" s="268" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="198"/>
+      <c r="M1" s="269"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
       <c r="A2" s="226">
         <v>1</v>
       </c>
-      <c r="B2" s="229" t="s">
+      <c r="B2" s="221" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -13416,145 +13416,145 @@
       <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="220" t="s">
+      <c r="E2" s="208" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="269"/>
-      <c r="G2" s="221"/>
-      <c r="H2" s="221"/>
-      <c r="I2" s="221" t="s">
+      <c r="F2" s="210"/>
+      <c r="G2" s="201"/>
+      <c r="H2" s="201"/>
+      <c r="I2" s="201" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="221" t="s">
+      <c r="J2" s="201" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="221" t="s">
+      <c r="K2" s="201" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="193" t="s">
+      <c r="L2" s="262" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="193" t="s">
+      <c r="M2" s="262" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A3" s="227"/>
-      <c r="B3" s="230"/>
+      <c r="A3" s="214"/>
+      <c r="B3" s="222"/>
       <c r="C3" s="32" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="215"/>
-      <c r="F3" s="242"/>
-      <c r="G3" s="212"/>
-      <c r="H3" s="212"/>
-      <c r="I3" s="212"/>
-      <c r="J3" s="212"/>
-      <c r="K3" s="212"/>
-      <c r="L3" s="190"/>
-      <c r="M3" s="190"/>
+      <c r="E3" s="203"/>
+      <c r="F3" s="211"/>
+      <c r="G3" s="197"/>
+      <c r="H3" s="197"/>
+      <c r="I3" s="197"/>
+      <c r="J3" s="197"/>
+      <c r="K3" s="197"/>
+      <c r="L3" s="245"/>
+      <c r="M3" s="245"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A4" s="227"/>
-      <c r="B4" s="230"/>
+      <c r="A4" s="214"/>
+      <c r="B4" s="222"/>
       <c r="C4" s="32" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="215"/>
-      <c r="F4" s="242"/>
-      <c r="G4" s="212"/>
-      <c r="H4" s="212"/>
-      <c r="I4" s="212"/>
-      <c r="J4" s="212"/>
-      <c r="K4" s="212"/>
-      <c r="L4" s="190"/>
-      <c r="M4" s="190"/>
+      <c r="E4" s="203"/>
+      <c r="F4" s="211"/>
+      <c r="G4" s="197"/>
+      <c r="H4" s="197"/>
+      <c r="I4" s="197"/>
+      <c r="J4" s="197"/>
+      <c r="K4" s="197"/>
+      <c r="L4" s="245"/>
+      <c r="M4" s="245"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A5" s="227"/>
-      <c r="B5" s="230"/>
+      <c r="A5" s="214"/>
+      <c r="B5" s="222"/>
       <c r="C5" s="32" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="215"/>
-      <c r="F5" s="242"/>
-      <c r="G5" s="212"/>
-      <c r="H5" s="212"/>
-      <c r="I5" s="212"/>
-      <c r="J5" s="212"/>
-      <c r="K5" s="212"/>
-      <c r="L5" s="190"/>
-      <c r="M5" s="190"/>
+      <c r="E5" s="203"/>
+      <c r="F5" s="211"/>
+      <c r="G5" s="197"/>
+      <c r="H5" s="197"/>
+      <c r="I5" s="197"/>
+      <c r="J5" s="197"/>
+      <c r="K5" s="197"/>
+      <c r="L5" s="245"/>
+      <c r="M5" s="245"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A6" s="227"/>
-      <c r="B6" s="230"/>
+      <c r="A6" s="214"/>
+      <c r="B6" s="222"/>
       <c r="C6" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="215"/>
-      <c r="F6" s="242"/>
-      <c r="G6" s="212"/>
-      <c r="H6" s="212"/>
-      <c r="I6" s="212"/>
-      <c r="J6" s="212"/>
-      <c r="K6" s="212"/>
-      <c r="L6" s="190"/>
-      <c r="M6" s="190"/>
+      <c r="E6" s="203"/>
+      <c r="F6" s="211"/>
+      <c r="G6" s="197"/>
+      <c r="H6" s="197"/>
+      <c r="I6" s="197"/>
+      <c r="J6" s="197"/>
+      <c r="K6" s="197"/>
+      <c r="L6" s="245"/>
+      <c r="M6" s="245"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A7" s="227"/>
-      <c r="B7" s="230"/>
+      <c r="A7" s="214"/>
+      <c r="B7" s="222"/>
       <c r="C7" s="32" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="215"/>
-      <c r="F7" s="242"/>
-      <c r="G7" s="212"/>
-      <c r="H7" s="212"/>
-      <c r="I7" s="212"/>
-      <c r="J7" s="212"/>
-      <c r="K7" s="212"/>
-      <c r="L7" s="190"/>
-      <c r="M7" s="190"/>
+      <c r="E7" s="203"/>
+      <c r="F7" s="211"/>
+      <c r="G7" s="197"/>
+      <c r="H7" s="197"/>
+      <c r="I7" s="197"/>
+      <c r="J7" s="197"/>
+      <c r="K7" s="197"/>
+      <c r="L7" s="245"/>
+      <c r="M7" s="245"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A8" s="228"/>
-      <c r="B8" s="231"/>
+      <c r="A8" s="215"/>
+      <c r="B8" s="223"/>
       <c r="C8" s="9" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="268"/>
-      <c r="F8" s="270"/>
-      <c r="G8" s="267"/>
-      <c r="H8" s="267"/>
-      <c r="I8" s="267"/>
-      <c r="J8" s="267"/>
-      <c r="K8" s="267"/>
-      <c r="L8" s="203"/>
-      <c r="M8" s="203"/>
+      <c r="E8" s="209"/>
+      <c r="F8" s="212"/>
+      <c r="G8" s="202"/>
+      <c r="H8" s="202"/>
+      <c r="I8" s="202"/>
+      <c r="J8" s="202"/>
+      <c r="K8" s="202"/>
+      <c r="L8" s="271"/>
+      <c r="M8" s="271"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A9" s="233">
+      <c r="A9" s="239">
         <v>2</v>
       </c>
-      <c r="B9" s="229" t="s">
+      <c r="B9" s="221" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -13563,864 +13563,864 @@
       <c r="D9" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="E9" s="246"/>
-      <c r="F9" s="225" t="s">
+      <c r="E9" s="204"/>
+      <c r="F9" s="205" t="s">
         <v>192</v>
       </c>
-      <c r="G9" s="240" t="s">
+      <c r="G9" s="207" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="224"/>
-      <c r="I9" s="244" t="s">
+      <c r="H9" s="248"/>
+      <c r="I9" s="249" t="s">
         <v>184</v>
       </c>
-      <c r="J9" s="225" t="s">
+      <c r="J9" s="205" t="s">
         <v>194</v>
       </c>
-      <c r="K9" s="225" t="s">
+      <c r="K9" s="205" t="s">
         <v>195</v>
       </c>
-      <c r="L9" s="240" t="s">
+      <c r="L9" s="207" t="s">
         <v>328</v>
       </c>
-      <c r="M9" s="204"/>
+      <c r="M9" s="272"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A10" s="234"/>
-      <c r="B10" s="230"/>
+      <c r="A10" s="237"/>
+      <c r="B10" s="222"/>
       <c r="C10" s="11" t="s">
         <v>26</v>
       </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="207"/>
-      <c r="F10" s="214"/>
-      <c r="G10" s="218"/>
-      <c r="H10" s="210"/>
-      <c r="I10" s="245"/>
-      <c r="J10" s="214"/>
-      <c r="K10" s="214"/>
-      <c r="L10" s="241"/>
-      <c r="M10" s="205"/>
+      <c r="E10" s="196"/>
+      <c r="F10" s="206"/>
+      <c r="G10" s="199"/>
+      <c r="H10" s="200"/>
+      <c r="I10" s="250"/>
+      <c r="J10" s="206"/>
+      <c r="K10" s="206"/>
+      <c r="L10" s="243"/>
+      <c r="M10" s="273"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A11" s="252">
+      <c r="A11" s="234">
         <v>3</v>
       </c>
-      <c r="B11" s="230"/>
+      <c r="B11" s="222"/>
       <c r="C11" s="11" t="s">
         <v>263</v>
       </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="215"/>
-      <c r="F11" s="242"/>
-      <c r="G11" s="212"/>
-      <c r="H11" s="212" t="s">
+      <c r="E11" s="203"/>
+      <c r="F11" s="211"/>
+      <c r="G11" s="197"/>
+      <c r="H11" s="197" t="s">
         <v>198</v>
       </c>
-      <c r="I11" s="212" t="s">
+      <c r="I11" s="197" t="s">
         <v>196</v>
       </c>
-      <c r="J11" s="212"/>
-      <c r="K11" s="212"/>
-      <c r="L11" s="239" t="s">
+      <c r="J11" s="197"/>
+      <c r="K11" s="197"/>
+      <c r="L11" s="242" t="s">
         <v>329</v>
       </c>
-      <c r="M11" s="190"/>
+      <c r="M11" s="245"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A12" s="253"/>
-      <c r="B12" s="230"/>
+      <c r="A12" s="235"/>
+      <c r="B12" s="222"/>
       <c r="C12" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D12" s="10"/>
-      <c r="E12" s="215"/>
-      <c r="F12" s="242"/>
-      <c r="G12" s="212"/>
-      <c r="H12" s="212"/>
-      <c r="I12" s="212"/>
-      <c r="J12" s="212"/>
-      <c r="K12" s="212"/>
-      <c r="L12" s="239"/>
-      <c r="M12" s="190"/>
+      <c r="E12" s="203"/>
+      <c r="F12" s="211"/>
+      <c r="G12" s="197"/>
+      <c r="H12" s="197"/>
+      <c r="I12" s="197"/>
+      <c r="J12" s="197"/>
+      <c r="K12" s="197"/>
+      <c r="L12" s="242"/>
+      <c r="M12" s="245"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A13" s="254">
+      <c r="A13" s="236">
         <v>4</v>
       </c>
-      <c r="B13" s="230"/>
+      <c r="B13" s="222"/>
       <c r="C13" s="11" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="11"/>
-      <c r="E13" s="207"/>
-      <c r="F13" s="266" t="s">
+      <c r="E13" s="196"/>
+      <c r="F13" s="198" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="218" t="s">
+      <c r="G13" s="199" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="210"/>
-      <c r="I13" s="218" t="s">
+      <c r="H13" s="200"/>
+      <c r="I13" s="199" t="s">
         <v>330</v>
       </c>
-      <c r="J13" s="210"/>
-      <c r="K13" s="210"/>
-      <c r="L13" s="191"/>
-      <c r="M13" s="191"/>
+      <c r="J13" s="200"/>
+      <c r="K13" s="200"/>
+      <c r="L13" s="263"/>
+      <c r="M13" s="263"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A14" s="234"/>
-      <c r="B14" s="230"/>
+      <c r="A14" s="237"/>
+      <c r="B14" s="222"/>
       <c r="C14" s="32" t="s">
         <v>30</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="207"/>
-      <c r="F14" s="266"/>
-      <c r="G14" s="218"/>
-      <c r="H14" s="210"/>
-      <c r="I14" s="218"/>
-      <c r="J14" s="210"/>
-      <c r="K14" s="210"/>
-      <c r="L14" s="191"/>
-      <c r="M14" s="191"/>
+      <c r="E14" s="196"/>
+      <c r="F14" s="198"/>
+      <c r="G14" s="199"/>
+      <c r="H14" s="200"/>
+      <c r="I14" s="199"/>
+      <c r="J14" s="200"/>
+      <c r="K14" s="200"/>
+      <c r="L14" s="263"/>
+      <c r="M14" s="263"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A15" s="252">
+      <c r="A15" s="234">
         <v>5</v>
       </c>
-      <c r="B15" s="230"/>
-      <c r="C15" s="237" t="s">
+      <c r="B15" s="222"/>
+      <c r="C15" s="240" t="s">
         <v>31</v>
       </c>
       <c r="D15" s="4"/>
-      <c r="E15" s="215" t="s">
+      <c r="E15" s="203" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="242"/>
-      <c r="G15" s="212"/>
-      <c r="H15" s="212"/>
-      <c r="I15" s="212"/>
-      <c r="J15" s="212"/>
-      <c r="K15" s="212"/>
-      <c r="L15" s="190"/>
-      <c r="M15" s="190"/>
+      <c r="F15" s="211"/>
+      <c r="G15" s="197"/>
+      <c r="H15" s="197"/>
+      <c r="I15" s="197"/>
+      <c r="J15" s="197"/>
+      <c r="K15" s="197"/>
+      <c r="L15" s="245"/>
+      <c r="M15" s="245"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A16" s="255"/>
-      <c r="B16" s="232"/>
-      <c r="C16" s="238"/>
+      <c r="A16" s="238"/>
+      <c r="B16" s="227"/>
+      <c r="C16" s="241"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="216"/>
-      <c r="F16" s="243"/>
-      <c r="G16" s="213"/>
-      <c r="H16" s="213"/>
-      <c r="I16" s="213"/>
-      <c r="J16" s="213"/>
-      <c r="K16" s="213"/>
-      <c r="L16" s="195"/>
-      <c r="M16" s="195"/>
+      <c r="E16" s="251"/>
+      <c r="F16" s="247"/>
+      <c r="G16" s="244"/>
+      <c r="H16" s="244"/>
+      <c r="I16" s="244"/>
+      <c r="J16" s="244"/>
+      <c r="K16" s="244"/>
+      <c r="L16" s="246"/>
+      <c r="M16" s="246"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A17" s="256">
+      <c r="A17" s="224">
         <v>6</v>
       </c>
-      <c r="B17" s="229" t="s">
+      <c r="B17" s="221" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>35</v>
       </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="246"/>
-      <c r="F17" s="224"/>
-      <c r="G17" s="224"/>
-      <c r="H17" s="225" t="s">
+      <c r="E17" s="204"/>
+      <c r="F17" s="248"/>
+      <c r="G17" s="248"/>
+      <c r="H17" s="205" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="225"/>
-      <c r="J17" s="225"/>
-      <c r="K17" s="225"/>
-      <c r="L17" s="199"/>
-      <c r="M17" s="199"/>
+      <c r="I17" s="205"/>
+      <c r="J17" s="205"/>
+      <c r="K17" s="205"/>
+      <c r="L17" s="270"/>
+      <c r="M17" s="270"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A18" s="235"/>
-      <c r="B18" s="230"/>
+      <c r="A18" s="213"/>
+      <c r="B18" s="222"/>
       <c r="C18" s="11" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="4"/>
-      <c r="E18" s="207"/>
-      <c r="F18" s="210"/>
-      <c r="G18" s="210"/>
-      <c r="H18" s="214"/>
-      <c r="I18" s="214"/>
-      <c r="J18" s="214"/>
-      <c r="K18" s="214"/>
-      <c r="L18" s="194"/>
-      <c r="M18" s="194"/>
+      <c r="E18" s="196"/>
+      <c r="F18" s="200"/>
+      <c r="G18" s="200"/>
+      <c r="H18" s="206"/>
+      <c r="I18" s="206"/>
+      <c r="J18" s="206"/>
+      <c r="K18" s="206"/>
+      <c r="L18" s="256"/>
+      <c r="M18" s="256"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A19" s="235"/>
-      <c r="B19" s="230"/>
+      <c r="A19" s="213"/>
+      <c r="B19" s="222"/>
       <c r="C19" s="11" t="s">
         <v>38</v>
       </c>
       <c r="D19" s="4"/>
-      <c r="E19" s="207"/>
-      <c r="F19" s="210"/>
-      <c r="G19" s="210"/>
-      <c r="H19" s="214"/>
-      <c r="I19" s="214"/>
-      <c r="J19" s="214"/>
-      <c r="K19" s="214"/>
-      <c r="L19" s="194"/>
-      <c r="M19" s="194"/>
+      <c r="E19" s="196"/>
+      <c r="F19" s="200"/>
+      <c r="G19" s="200"/>
+      <c r="H19" s="206"/>
+      <c r="I19" s="206"/>
+      <c r="J19" s="206"/>
+      <c r="K19" s="206"/>
+      <c r="L19" s="256"/>
+      <c r="M19" s="256"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A20" s="227">
+      <c r="A20" s="214">
         <v>7</v>
       </c>
-      <c r="B20" s="230"/>
+      <c r="B20" s="222"/>
       <c r="C20" s="11" t="s">
         <v>39</v>
       </c>
       <c r="D20" s="4"/>
-      <c r="E20" s="215" t="s">
+      <c r="E20" s="203" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="223" t="s">
+      <c r="F20" s="258" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="223"/>
-      <c r="H20" s="223"/>
-      <c r="I20" s="223"/>
-      <c r="J20" s="223"/>
-      <c r="K20" s="223"/>
-      <c r="L20" s="200"/>
-      <c r="M20" s="200"/>
+      <c r="G20" s="258"/>
+      <c r="H20" s="258"/>
+      <c r="I20" s="258"/>
+      <c r="J20" s="258"/>
+      <c r="K20" s="258"/>
+      <c r="L20" s="259"/>
+      <c r="M20" s="259"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A21" s="227"/>
-      <c r="B21" s="230"/>
+      <c r="A21" s="214"/>
+      <c r="B21" s="222"/>
       <c r="C21" s="11" t="s">
         <v>41</v>
       </c>
       <c r="D21" s="4"/>
-      <c r="E21" s="215"/>
-      <c r="F21" s="223"/>
-      <c r="G21" s="223"/>
-      <c r="H21" s="223"/>
-      <c r="I21" s="223"/>
-      <c r="J21" s="223"/>
-      <c r="K21" s="223"/>
-      <c r="L21" s="200"/>
-      <c r="M21" s="200"/>
+      <c r="E21" s="203"/>
+      <c r="F21" s="258"/>
+      <c r="G21" s="258"/>
+      <c r="H21" s="258"/>
+      <c r="I21" s="258"/>
+      <c r="J21" s="258"/>
+      <c r="K21" s="258"/>
+      <c r="L21" s="259"/>
+      <c r="M21" s="259"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A22" s="227"/>
-      <c r="B22" s="230"/>
+      <c r="A22" s="214"/>
+      <c r="B22" s="222"/>
       <c r="C22" s="32" t="s">
         <v>42</v>
       </c>
       <c r="D22" s="4"/>
-      <c r="E22" s="215"/>
-      <c r="F22" s="223"/>
-      <c r="G22" s="223"/>
-      <c r="H22" s="223"/>
-      <c r="I22" s="223"/>
-      <c r="J22" s="223"/>
-      <c r="K22" s="223"/>
-      <c r="L22" s="200"/>
-      <c r="M22" s="200"/>
+      <c r="E22" s="203"/>
+      <c r="F22" s="258"/>
+      <c r="G22" s="258"/>
+      <c r="H22" s="258"/>
+      <c r="I22" s="258"/>
+      <c r="J22" s="258"/>
+      <c r="K22" s="258"/>
+      <c r="L22" s="259"/>
+      <c r="M22" s="259"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A23" s="235">
+      <c r="A23" s="213">
         <v>8</v>
       </c>
-      <c r="B23" s="230"/>
+      <c r="B23" s="222"/>
       <c r="C23" s="32" t="s">
         <v>43</v>
       </c>
       <c r="D23" s="4"/>
-      <c r="E23" s="207"/>
-      <c r="F23" s="210"/>
-      <c r="G23" s="218" t="s">
+      <c r="E23" s="196"/>
+      <c r="F23" s="200"/>
+      <c r="G23" s="199" t="s">
         <v>50</v>
       </c>
-      <c r="H23" s="214" t="s">
+      <c r="H23" s="206" t="s">
         <v>32</v>
       </c>
-      <c r="I23" s="214"/>
-      <c r="J23" s="214"/>
-      <c r="K23" s="214"/>
-      <c r="L23" s="194"/>
-      <c r="M23" s="194"/>
+      <c r="I23" s="206"/>
+      <c r="J23" s="206"/>
+      <c r="K23" s="206"/>
+      <c r="L23" s="256"/>
+      <c r="M23" s="256"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A24" s="235"/>
-      <c r="B24" s="230"/>
+      <c r="A24" s="213"/>
+      <c r="B24" s="222"/>
       <c r="C24" s="32" t="s">
         <v>45</v>
       </c>
       <c r="D24" s="4"/>
-      <c r="E24" s="207"/>
-      <c r="F24" s="210"/>
-      <c r="G24" s="218"/>
-      <c r="H24" s="214"/>
-      <c r="I24" s="214"/>
-      <c r="J24" s="214"/>
-      <c r="K24" s="214"/>
-      <c r="L24" s="194"/>
-      <c r="M24" s="194"/>
+      <c r="E24" s="196"/>
+      <c r="F24" s="200"/>
+      <c r="G24" s="199"/>
+      <c r="H24" s="206"/>
+      <c r="I24" s="206"/>
+      <c r="J24" s="206"/>
+      <c r="K24" s="206"/>
+      <c r="L24" s="256"/>
+      <c r="M24" s="256"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A25" s="236"/>
-      <c r="B25" s="232"/>
+      <c r="A25" s="230"/>
+      <c r="B25" s="227"/>
       <c r="C25" s="33" t="s">
         <v>46</v>
       </c>
       <c r="D25" s="5"/>
-      <c r="E25" s="208"/>
-      <c r="F25" s="211"/>
-      <c r="G25" s="219"/>
-      <c r="H25" s="217"/>
-      <c r="I25" s="217"/>
-      <c r="J25" s="217"/>
-      <c r="K25" s="217"/>
-      <c r="L25" s="201"/>
-      <c r="M25" s="201"/>
+      <c r="E25" s="252"/>
+      <c r="F25" s="253"/>
+      <c r="G25" s="254"/>
+      <c r="H25" s="255"/>
+      <c r="I25" s="255"/>
+      <c r="J25" s="255"/>
+      <c r="K25" s="255"/>
+      <c r="L25" s="257"/>
+      <c r="M25" s="257"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A26" s="247">
+      <c r="A26" s="228">
         <v>9</v>
       </c>
-      <c r="B26" s="229" t="s">
+      <c r="B26" s="221" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>48</v>
       </c>
       <c r="D26" s="3"/>
-      <c r="E26" s="220" t="s">
+      <c r="E26" s="208" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="222" t="s">
+      <c r="F26" s="260" t="s">
         <v>53</v>
       </c>
-      <c r="G26" s="222"/>
-      <c r="H26" s="222"/>
-      <c r="I26" s="222"/>
-      <c r="J26" s="222"/>
-      <c r="K26" s="222"/>
-      <c r="L26" s="202"/>
-      <c r="M26" s="202"/>
+      <c r="G26" s="260"/>
+      <c r="H26" s="260"/>
+      <c r="I26" s="260"/>
+      <c r="J26" s="260"/>
+      <c r="K26" s="260"/>
+      <c r="L26" s="261"/>
+      <c r="M26" s="261"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A27" s="248"/>
-      <c r="B27" s="230"/>
+      <c r="A27" s="229"/>
+      <c r="B27" s="222"/>
       <c r="C27" s="13" t="s">
         <v>51</v>
       </c>
       <c r="D27" s="4"/>
-      <c r="E27" s="215"/>
-      <c r="F27" s="223"/>
-      <c r="G27" s="223"/>
-      <c r="H27" s="223"/>
-      <c r="I27" s="223"/>
-      <c r="J27" s="223"/>
-      <c r="K27" s="223"/>
-      <c r="L27" s="200"/>
-      <c r="M27" s="200"/>
+      <c r="E27" s="203"/>
+      <c r="F27" s="258"/>
+      <c r="G27" s="258"/>
+      <c r="H27" s="258"/>
+      <c r="I27" s="258"/>
+      <c r="J27" s="258"/>
+      <c r="K27" s="258"/>
+      <c r="L27" s="259"/>
+      <c r="M27" s="259"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A28" s="236">
+      <c r="A28" s="230">
         <v>10</v>
       </c>
-      <c r="B28" s="230"/>
+      <c r="B28" s="222"/>
       <c r="C28" s="13" t="s">
         <v>52</v>
       </c>
       <c r="D28" s="4"/>
-      <c r="E28" s="207"/>
-      <c r="F28" s="214" t="s">
+      <c r="E28" s="196"/>
+      <c r="F28" s="206" t="s">
         <v>59</v>
       </c>
-      <c r="G28" s="214"/>
-      <c r="H28" s="214" t="s">
+      <c r="G28" s="206"/>
+      <c r="H28" s="206" t="s">
         <v>40</v>
       </c>
-      <c r="I28" s="214"/>
-      <c r="J28" s="214"/>
-      <c r="K28" s="214"/>
-      <c r="L28" s="194"/>
-      <c r="M28" s="194"/>
+      <c r="I28" s="206"/>
+      <c r="J28" s="206"/>
+      <c r="K28" s="206"/>
+      <c r="L28" s="256"/>
+      <c r="M28" s="256"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A29" s="249"/>
-      <c r="B29" s="230"/>
+      <c r="A29" s="231"/>
+      <c r="B29" s="222"/>
       <c r="C29" s="13" t="s">
         <v>54</v>
       </c>
       <c r="D29" s="4"/>
-      <c r="E29" s="207"/>
-      <c r="F29" s="214"/>
-      <c r="G29" s="214"/>
-      <c r="H29" s="214"/>
-      <c r="I29" s="214"/>
-      <c r="J29" s="214"/>
-      <c r="K29" s="214"/>
-      <c r="L29" s="194"/>
-      <c r="M29" s="194"/>
+      <c r="E29" s="196"/>
+      <c r="F29" s="206"/>
+      <c r="G29" s="206"/>
+      <c r="H29" s="206"/>
+      <c r="I29" s="206"/>
+      <c r="J29" s="206"/>
+      <c r="K29" s="206"/>
+      <c r="L29" s="256"/>
+      <c r="M29" s="256"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A30" s="250">
+      <c r="A30" s="232">
         <v>11</v>
       </c>
-      <c r="B30" s="230"/>
+      <c r="B30" s="222"/>
       <c r="C30" s="13" t="s">
         <v>55</v>
       </c>
       <c r="D30" s="4"/>
-      <c r="E30" s="215" t="s">
+      <c r="E30" s="203" t="s">
         <v>49</v>
       </c>
-      <c r="F30" s="212"/>
-      <c r="G30" s="212"/>
-      <c r="H30" s="212"/>
-      <c r="I30" s="212"/>
-      <c r="J30" s="212"/>
-      <c r="K30" s="212"/>
-      <c r="L30" s="190"/>
-      <c r="M30" s="190"/>
+      <c r="F30" s="197"/>
+      <c r="G30" s="197"/>
+      <c r="H30" s="197"/>
+      <c r="I30" s="197"/>
+      <c r="J30" s="197"/>
+      <c r="K30" s="197"/>
+      <c r="L30" s="245"/>
+      <c r="M30" s="245"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A31" s="248"/>
-      <c r="B31" s="230"/>
+      <c r="A31" s="229"/>
+      <c r="B31" s="222"/>
       <c r="C31" s="14" t="s">
         <v>57</v>
       </c>
       <c r="D31" s="4"/>
-      <c r="E31" s="215"/>
-      <c r="F31" s="212"/>
-      <c r="G31" s="212"/>
-      <c r="H31" s="212"/>
-      <c r="I31" s="212"/>
-      <c r="J31" s="212"/>
-      <c r="K31" s="212"/>
-      <c r="L31" s="190"/>
-      <c r="M31" s="190"/>
+      <c r="E31" s="203"/>
+      <c r="F31" s="197"/>
+      <c r="G31" s="197"/>
+      <c r="H31" s="197"/>
+      <c r="I31" s="197"/>
+      <c r="J31" s="197"/>
+      <c r="K31" s="197"/>
+      <c r="L31" s="245"/>
+      <c r="M31" s="245"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A32" s="236">
+      <c r="A32" s="230">
         <v>12</v>
       </c>
-      <c r="B32" s="230"/>
+      <c r="B32" s="222"/>
       <c r="C32" s="14" t="s">
         <v>58</v>
       </c>
       <c r="D32" s="4"/>
-      <c r="E32" s="207"/>
-      <c r="F32" s="214" t="s">
+      <c r="E32" s="196"/>
+      <c r="F32" s="206" t="s">
         <v>67</v>
       </c>
-      <c r="G32" s="218" t="s">
+      <c r="G32" s="199" t="s">
         <v>64</v>
       </c>
-      <c r="H32" s="214" t="s">
+      <c r="H32" s="206" t="s">
         <v>49</v>
       </c>
-      <c r="I32" s="214"/>
-      <c r="J32" s="214"/>
-      <c r="K32" s="214"/>
-      <c r="L32" s="194"/>
-      <c r="M32" s="194"/>
+      <c r="I32" s="206"/>
+      <c r="J32" s="206"/>
+      <c r="K32" s="206"/>
+      <c r="L32" s="256"/>
+      <c r="M32" s="256"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A33" s="251"/>
-      <c r="B33" s="232"/>
+      <c r="A33" s="233"/>
+      <c r="B33" s="227"/>
       <c r="C33" s="15" t="s">
         <v>60</v>
       </c>
       <c r="D33" s="5"/>
-      <c r="E33" s="208"/>
-      <c r="F33" s="217"/>
-      <c r="G33" s="219"/>
-      <c r="H33" s="217"/>
-      <c r="I33" s="217"/>
-      <c r="J33" s="217"/>
-      <c r="K33" s="217"/>
-      <c r="L33" s="201"/>
-      <c r="M33" s="201"/>
+      <c r="E33" s="252"/>
+      <c r="F33" s="255"/>
+      <c r="G33" s="254"/>
+      <c r="H33" s="255"/>
+      <c r="I33" s="255"/>
+      <c r="J33" s="255"/>
+      <c r="K33" s="255"/>
+      <c r="L33" s="257"/>
+      <c r="M33" s="257"/>
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1">
       <c r="A34" s="226">
         <v>13</v>
       </c>
-      <c r="B34" s="229" t="s">
+      <c r="B34" s="221" t="s">
         <v>61</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>62</v>
       </c>
       <c r="D34" s="3"/>
-      <c r="E34" s="220" t="s">
+      <c r="E34" s="208" t="s">
         <v>56</v>
       </c>
-      <c r="F34" s="221"/>
-      <c r="G34" s="221"/>
-      <c r="H34" s="221"/>
-      <c r="I34" s="221"/>
-      <c r="J34" s="221"/>
-      <c r="K34" s="221"/>
-      <c r="L34" s="193"/>
-      <c r="M34" s="193"/>
+      <c r="F34" s="201"/>
+      <c r="G34" s="201"/>
+      <c r="H34" s="201"/>
+      <c r="I34" s="201"/>
+      <c r="J34" s="201"/>
+      <c r="K34" s="201"/>
+      <c r="L34" s="262"/>
+      <c r="M34" s="262"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A35" s="227"/>
-      <c r="B35" s="230"/>
+      <c r="A35" s="214"/>
+      <c r="B35" s="222"/>
       <c r="C35" s="17" t="s">
         <v>65</v>
       </c>
       <c r="D35" s="4"/>
-      <c r="E35" s="215"/>
-      <c r="F35" s="212"/>
-      <c r="G35" s="212"/>
-      <c r="H35" s="212"/>
-      <c r="I35" s="212"/>
-      <c r="J35" s="212"/>
-      <c r="K35" s="212"/>
-      <c r="L35" s="190"/>
-      <c r="M35" s="190"/>
+      <c r="E35" s="203"/>
+      <c r="F35" s="197"/>
+      <c r="G35" s="197"/>
+      <c r="H35" s="197"/>
+      <c r="I35" s="197"/>
+      <c r="J35" s="197"/>
+      <c r="K35" s="197"/>
+      <c r="L35" s="245"/>
+      <c r="M35" s="245"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A36" s="235">
+      <c r="A36" s="213">
         <v>14</v>
       </c>
-      <c r="B36" s="230"/>
+      <c r="B36" s="222"/>
       <c r="C36" s="17" t="s">
         <v>66</v>
       </c>
       <c r="D36" s="4"/>
-      <c r="E36" s="207"/>
-      <c r="F36" s="210" t="s">
+      <c r="E36" s="196"/>
+      <c r="F36" s="200" t="s">
         <v>73</v>
       </c>
-      <c r="G36" s="210"/>
-      <c r="H36" s="210" t="s">
+      <c r="G36" s="200"/>
+      <c r="H36" s="200" t="s">
         <v>56</v>
       </c>
-      <c r="I36" s="210"/>
-      <c r="J36" s="210"/>
-      <c r="K36" s="210"/>
-      <c r="L36" s="191"/>
-      <c r="M36" s="191"/>
+      <c r="I36" s="200"/>
+      <c r="J36" s="200"/>
+      <c r="K36" s="200"/>
+      <c r="L36" s="263"/>
+      <c r="M36" s="263"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A37" s="235"/>
-      <c r="B37" s="230"/>
+      <c r="A37" s="213"/>
+      <c r="B37" s="222"/>
       <c r="C37" s="17" t="s">
         <v>68</v>
       </c>
       <c r="D37" s="4"/>
-      <c r="E37" s="207"/>
-      <c r="F37" s="210"/>
-      <c r="G37" s="210"/>
-      <c r="H37" s="210"/>
-      <c r="I37" s="210"/>
-      <c r="J37" s="210"/>
-      <c r="K37" s="210"/>
-      <c r="L37" s="191"/>
-      <c r="M37" s="191"/>
+      <c r="E37" s="196"/>
+      <c r="F37" s="200"/>
+      <c r="G37" s="200"/>
+      <c r="H37" s="200"/>
+      <c r="I37" s="200"/>
+      <c r="J37" s="200"/>
+      <c r="K37" s="200"/>
+      <c r="L37" s="263"/>
+      <c r="M37" s="263"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A38" s="227">
+      <c r="A38" s="214">
         <v>15</v>
       </c>
-      <c r="B38" s="230"/>
+      <c r="B38" s="222"/>
       <c r="C38" s="17" t="s">
         <v>69</v>
       </c>
       <c r="D38" s="4"/>
-      <c r="E38" s="215" t="s">
+      <c r="E38" s="203" t="s">
         <v>63</v>
       </c>
-      <c r="F38" s="212"/>
-      <c r="G38" s="212"/>
-      <c r="H38" s="212"/>
-      <c r="I38" s="212"/>
-      <c r="J38" s="212"/>
-      <c r="K38" s="212"/>
-      <c r="L38" s="190"/>
-      <c r="M38" s="190"/>
+      <c r="F38" s="197"/>
+      <c r="G38" s="197"/>
+      <c r="H38" s="197"/>
+      <c r="I38" s="197"/>
+      <c r="J38" s="197"/>
+      <c r="K38" s="197"/>
+      <c r="L38" s="245"/>
+      <c r="M38" s="245"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A39" s="227"/>
-      <c r="B39" s="230"/>
+      <c r="A39" s="214"/>
+      <c r="B39" s="222"/>
       <c r="C39" s="32" t="s">
         <v>71</v>
       </c>
       <c r="D39" s="4"/>
-      <c r="E39" s="215"/>
-      <c r="F39" s="212"/>
-      <c r="G39" s="212"/>
-      <c r="H39" s="212"/>
-      <c r="I39" s="212"/>
-      <c r="J39" s="212"/>
-      <c r="K39" s="212"/>
-      <c r="L39" s="190"/>
-      <c r="M39" s="190"/>
+      <c r="E39" s="203"/>
+      <c r="F39" s="197"/>
+      <c r="G39" s="197"/>
+      <c r="H39" s="197"/>
+      <c r="I39" s="197"/>
+      <c r="J39" s="197"/>
+      <c r="K39" s="197"/>
+      <c r="L39" s="245"/>
+      <c r="M39" s="245"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A40" s="235">
+      <c r="A40" s="213">
         <v>16</v>
       </c>
-      <c r="B40" s="230"/>
+      <c r="B40" s="222"/>
       <c r="C40" s="32" t="s">
         <v>72</v>
       </c>
       <c r="D40" s="4"/>
-      <c r="E40" s="207"/>
-      <c r="F40" s="214" t="s">
+      <c r="E40" s="196"/>
+      <c r="F40" s="206" t="s">
         <v>82</v>
       </c>
-      <c r="G40" s="218" t="s">
+      <c r="G40" s="199" t="s">
         <v>79</v>
       </c>
-      <c r="H40" s="210" t="s">
+      <c r="H40" s="200" t="s">
         <v>63</v>
       </c>
-      <c r="I40" s="210"/>
-      <c r="J40" s="210"/>
-      <c r="K40" s="210"/>
-      <c r="L40" s="191"/>
-      <c r="M40" s="191"/>
+      <c r="I40" s="200"/>
+      <c r="J40" s="200"/>
+      <c r="K40" s="200"/>
+      <c r="L40" s="263"/>
+      <c r="M40" s="263"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A41" s="235"/>
-      <c r="B41" s="230"/>
+      <c r="A41" s="213"/>
+      <c r="B41" s="222"/>
       <c r="C41" s="32" t="s">
         <v>74</v>
       </c>
       <c r="D41" s="4"/>
-      <c r="E41" s="207"/>
-      <c r="F41" s="214"/>
-      <c r="G41" s="218"/>
-      <c r="H41" s="210"/>
-      <c r="I41" s="210"/>
-      <c r="J41" s="210"/>
-      <c r="K41" s="210"/>
-      <c r="L41" s="191"/>
-      <c r="M41" s="191"/>
+      <c r="E41" s="196"/>
+      <c r="F41" s="206"/>
+      <c r="G41" s="199"/>
+      <c r="H41" s="200"/>
+      <c r="I41" s="200"/>
+      <c r="J41" s="200"/>
+      <c r="K41" s="200"/>
+      <c r="L41" s="263"/>
+      <c r="M41" s="263"/>
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A42" s="262"/>
-      <c r="B42" s="231"/>
+      <c r="A42" s="225"/>
+      <c r="B42" s="223"/>
       <c r="C42" s="9" t="s">
         <v>75</v>
       </c>
       <c r="D42" s="5"/>
-      <c r="E42" s="208"/>
-      <c r="F42" s="217"/>
-      <c r="G42" s="219"/>
-      <c r="H42" s="211"/>
-      <c r="I42" s="211"/>
-      <c r="J42" s="211"/>
-      <c r="K42" s="211"/>
-      <c r="L42" s="192"/>
-      <c r="M42" s="192"/>
+      <c r="E42" s="252"/>
+      <c r="F42" s="255"/>
+      <c r="G42" s="254"/>
+      <c r="H42" s="253"/>
+      <c r="I42" s="253"/>
+      <c r="J42" s="253"/>
+      <c r="K42" s="253"/>
+      <c r="L42" s="264"/>
+      <c r="M42" s="264"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" customHeight="1">
       <c r="A43" s="226">
         <v>17</v>
       </c>
-      <c r="B43" s="257" t="s">
+      <c r="B43" s="216" t="s">
         <v>76</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>77</v>
       </c>
       <c r="D43" s="3"/>
-      <c r="E43" s="220" t="s">
+      <c r="E43" s="208" t="s">
         <v>70</v>
       </c>
-      <c r="F43" s="221"/>
-      <c r="G43" s="221"/>
-      <c r="H43" s="221"/>
-      <c r="I43" s="221"/>
-      <c r="J43" s="221"/>
-      <c r="K43" s="221"/>
-      <c r="L43" s="193"/>
-      <c r="M43" s="193"/>
+      <c r="F43" s="201"/>
+      <c r="G43" s="201"/>
+      <c r="H43" s="201"/>
+      <c r="I43" s="201"/>
+      <c r="J43" s="201"/>
+      <c r="K43" s="201"/>
+      <c r="L43" s="262"/>
+      <c r="M43" s="262"/>
     </row>
     <row r="44" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A44" s="227"/>
-      <c r="B44" s="258"/>
+      <c r="A44" s="214"/>
+      <c r="B44" s="217"/>
       <c r="C44" s="11" t="s">
         <v>80</v>
       </c>
       <c r="D44" s="4"/>
-      <c r="E44" s="215"/>
-      <c r="F44" s="212"/>
-      <c r="G44" s="212"/>
-      <c r="H44" s="212"/>
-      <c r="I44" s="212"/>
-      <c r="J44" s="212"/>
-      <c r="K44" s="212"/>
-      <c r="L44" s="190"/>
-      <c r="M44" s="190"/>
+      <c r="E44" s="203"/>
+      <c r="F44" s="197"/>
+      <c r="G44" s="197"/>
+      <c r="H44" s="197"/>
+      <c r="I44" s="197"/>
+      <c r="J44" s="197"/>
+      <c r="K44" s="197"/>
+      <c r="L44" s="245"/>
+      <c r="M44" s="245"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A45" s="235">
+      <c r="A45" s="213">
         <v>18</v>
       </c>
-      <c r="B45" s="258"/>
+      <c r="B45" s="217"/>
       <c r="C45" s="11" t="s">
         <v>81</v>
       </c>
       <c r="D45" s="4"/>
-      <c r="E45" s="207"/>
-      <c r="F45" s="214" t="s">
+      <c r="E45" s="196"/>
+      <c r="F45" s="206" t="s">
         <v>197</v>
       </c>
-      <c r="G45" s="210"/>
-      <c r="H45" s="214" t="s">
+      <c r="G45" s="200"/>
+      <c r="H45" s="206" t="s">
         <v>70</v>
       </c>
-      <c r="I45" s="214"/>
-      <c r="J45" s="214"/>
-      <c r="K45" s="214"/>
-      <c r="L45" s="194"/>
-      <c r="M45" s="194"/>
+      <c r="I45" s="206"/>
+      <c r="J45" s="206"/>
+      <c r="K45" s="206"/>
+      <c r="L45" s="256"/>
+      <c r="M45" s="256"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A46" s="235"/>
-      <c r="B46" s="258"/>
+      <c r="A46" s="213"/>
+      <c r="B46" s="217"/>
       <c r="C46" s="11" t="s">
         <v>83</v>
       </c>
       <c r="D46" s="4"/>
-      <c r="E46" s="207"/>
-      <c r="F46" s="214"/>
-      <c r="G46" s="210"/>
-      <c r="H46" s="214"/>
-      <c r="I46" s="214"/>
-      <c r="J46" s="214"/>
-      <c r="K46" s="214"/>
-      <c r="L46" s="194"/>
-      <c r="M46" s="194"/>
+      <c r="E46" s="196"/>
+      <c r="F46" s="206"/>
+      <c r="G46" s="200"/>
+      <c r="H46" s="206"/>
+      <c r="I46" s="206"/>
+      <c r="J46" s="206"/>
+      <c r="K46" s="206"/>
+      <c r="L46" s="256"/>
+      <c r="M46" s="256"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A47" s="227">
+      <c r="A47" s="214">
         <v>19</v>
       </c>
-      <c r="B47" s="258"/>
-      <c r="C47" s="260" t="s">
+      <c r="B47" s="217"/>
+      <c r="C47" s="219" t="s">
         <v>84</v>
       </c>
       <c r="D47" s="4"/>
-      <c r="E47" s="215" t="s">
+      <c r="E47" s="203" t="s">
         <v>78</v>
       </c>
-      <c r="F47" s="212"/>
-      <c r="G47" s="212"/>
-      <c r="H47" s="212"/>
-      <c r="I47" s="212"/>
-      <c r="J47" s="212"/>
-      <c r="K47" s="212"/>
-      <c r="L47" s="190"/>
-      <c r="M47" s="190"/>
+      <c r="F47" s="197"/>
+      <c r="G47" s="197"/>
+      <c r="H47" s="197"/>
+      <c r="I47" s="197"/>
+      <c r="J47" s="197"/>
+      <c r="K47" s="197"/>
+      <c r="L47" s="245"/>
+      <c r="M47" s="245"/>
     </row>
     <row r="48" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A48" s="228"/>
-      <c r="B48" s="259"/>
-      <c r="C48" s="261"/>
+      <c r="A48" s="215"/>
+      <c r="B48" s="218"/>
+      <c r="C48" s="220"/>
       <c r="D48" s="5"/>
-      <c r="E48" s="216"/>
-      <c r="F48" s="213"/>
-      <c r="G48" s="213"/>
-      <c r="H48" s="213"/>
-      <c r="I48" s="213"/>
-      <c r="J48" s="213"/>
-      <c r="K48" s="213"/>
-      <c r="L48" s="195"/>
-      <c r="M48" s="195"/>
+      <c r="E48" s="251"/>
+      <c r="F48" s="244"/>
+      <c r="G48" s="244"/>
+      <c r="H48" s="244"/>
+      <c r="I48" s="244"/>
+      <c r="J48" s="244"/>
+      <c r="K48" s="244"/>
+      <c r="L48" s="246"/>
+      <c r="M48" s="246"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A49" s="256">
+      <c r="A49" s="224">
         <v>20</v>
       </c>
-      <c r="B49" s="229" t="s">
+      <c r="B49" s="221" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>86</v>
       </c>
       <c r="D49" s="6"/>
-      <c r="E49" s="206"/>
-      <c r="F49" s="209"/>
-      <c r="G49" s="209"/>
-      <c r="H49" s="209" t="s">
+      <c r="E49" s="265"/>
+      <c r="F49" s="266"/>
+      <c r="G49" s="266"/>
+      <c r="H49" s="266" t="s">
         <v>78</v>
       </c>
-      <c r="I49" s="209"/>
-      <c r="J49" s="209"/>
-      <c r="K49" s="209"/>
-      <c r="L49" s="196"/>
-      <c r="M49" s="196"/>
+      <c r="I49" s="266"/>
+      <c r="J49" s="266"/>
+      <c r="K49" s="266"/>
+      <c r="L49" s="267"/>
+      <c r="M49" s="267"/>
     </row>
     <row r="50" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A50" s="235"/>
-      <c r="B50" s="230"/>
+      <c r="A50" s="213"/>
+      <c r="B50" s="222"/>
       <c r="C50" s="11" t="s">
         <v>87</v>
       </c>
       <c r="D50" s="4"/>
-      <c r="E50" s="207"/>
-      <c r="F50" s="210"/>
-      <c r="G50" s="210"/>
-      <c r="H50" s="210"/>
-      <c r="I50" s="210"/>
-      <c r="J50" s="210"/>
-      <c r="K50" s="210"/>
-      <c r="L50" s="191"/>
-      <c r="M50" s="191"/>
+      <c r="E50" s="196"/>
+      <c r="F50" s="200"/>
+      <c r="G50" s="200"/>
+      <c r="H50" s="200"/>
+      <c r="I50" s="200"/>
+      <c r="J50" s="200"/>
+      <c r="K50" s="200"/>
+      <c r="L50" s="263"/>
+      <c r="M50" s="263"/>
     </row>
     <row r="51" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A51" s="235"/>
-      <c r="B51" s="230"/>
+      <c r="A51" s="213"/>
+      <c r="B51" s="222"/>
       <c r="C51" s="11" t="s">
         <v>88</v>
       </c>
       <c r="D51" s="4"/>
-      <c r="E51" s="207"/>
-      <c r="F51" s="210"/>
-      <c r="G51" s="210"/>
-      <c r="H51" s="210"/>
-      <c r="I51" s="210"/>
-      <c r="J51" s="210"/>
-      <c r="K51" s="210"/>
-      <c r="L51" s="191"/>
-      <c r="M51" s="191"/>
+      <c r="E51" s="196"/>
+      <c r="F51" s="200"/>
+      <c r="G51" s="200"/>
+      <c r="H51" s="200"/>
+      <c r="I51" s="200"/>
+      <c r="J51" s="200"/>
+      <c r="K51" s="200"/>
+      <c r="L51" s="263"/>
+      <c r="M51" s="263"/>
     </row>
     <row r="52" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A52" s="262"/>
-      <c r="B52" s="231"/>
+      <c r="A52" s="225"/>
+      <c r="B52" s="223"/>
       <c r="C52" s="18" t="s">
         <v>89</v>
       </c>
       <c r="D52" s="5"/>
-      <c r="E52" s="208"/>
-      <c r="F52" s="211"/>
-      <c r="G52" s="211"/>
-      <c r="H52" s="211"/>
-      <c r="I52" s="211"/>
-      <c r="J52" s="211"/>
-      <c r="K52" s="211"/>
-      <c r="L52" s="192"/>
-      <c r="M52" s="192"/>
+      <c r="E52" s="252"/>
+      <c r="F52" s="253"/>
+      <c r="G52" s="253"/>
+      <c r="H52" s="253"/>
+      <c r="I52" s="253"/>
+      <c r="J52" s="253"/>
+      <c r="K52" s="253"/>
+      <c r="L52" s="264"/>
+      <c r="M52" s="264"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="56" spans="1:13" ht="15.75" thickBot="1">
@@ -14491,49 +14491,150 @@
     </row>
   </sheetData>
   <mergeCells count="211">
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="J2:J8"/>
-    <mergeCell ref="K2:K8"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="E2:E8"/>
-    <mergeCell ref="F2:F8"/>
-    <mergeCell ref="G2:G8"/>
-    <mergeCell ref="H2:H8"/>
-    <mergeCell ref="I2:I8"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B43:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B34:B42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B26:B33"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="M40:M42"/>
+    <mergeCell ref="M43:M44"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="M47:M48"/>
+    <mergeCell ref="M49:M52"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="M17:M19"/>
+    <mergeCell ref="M20:M22"/>
+    <mergeCell ref="M23:M25"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="M32:M33"/>
+    <mergeCell ref="M34:M35"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="M2:M8"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="L17:L19"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="L2:L8"/>
+    <mergeCell ref="E49:E52"/>
+    <mergeCell ref="F49:F52"/>
+    <mergeCell ref="G49:G52"/>
+    <mergeCell ref="H49:H52"/>
+    <mergeCell ref="I49:I52"/>
+    <mergeCell ref="J49:J52"/>
+    <mergeCell ref="K49:K52"/>
+    <mergeCell ref="L49:L52"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="I47:I48"/>
+    <mergeCell ref="J47:J48"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="I45:I46"/>
+    <mergeCell ref="J45:J46"/>
+    <mergeCell ref="K45:K46"/>
+    <mergeCell ref="L45:L46"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="K47:K48"/>
+    <mergeCell ref="L47:L48"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="H40:H42"/>
+    <mergeCell ref="I40:I42"/>
+    <mergeCell ref="J40:J42"/>
+    <mergeCell ref="K40:K42"/>
+    <mergeCell ref="L40:L42"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="K43:K44"/>
+    <mergeCell ref="L43:L44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="I43:I44"/>
+    <mergeCell ref="J43:J44"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="K38:K39"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="K34:K35"/>
+    <mergeCell ref="L34:L35"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="K36:K37"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="L32:L33"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="L23:L25"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="I20:I22"/>
+    <mergeCell ref="J20:J22"/>
+    <mergeCell ref="K20:K22"/>
+    <mergeCell ref="L20:L22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="I17:I19"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="K17:K19"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="I23:I25"/>
+    <mergeCell ref="J23:J25"/>
+    <mergeCell ref="K23:K25"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="B2:B8"/>
     <mergeCell ref="B9:B16"/>
@@ -14558,150 +14659,49 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="E17:E19"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="I17:I19"/>
-    <mergeCell ref="J17:J19"/>
-    <mergeCell ref="K17:K19"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="I23:I25"/>
-    <mergeCell ref="J23:J25"/>
-    <mergeCell ref="K23:K25"/>
-    <mergeCell ref="L23:L25"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="I20:I22"/>
-    <mergeCell ref="J20:J22"/>
-    <mergeCell ref="K20:K22"/>
-    <mergeCell ref="L20:L22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="L30:L31"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="L28:L29"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="L32:L33"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="J34:J35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="K38:K39"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="K34:K35"/>
-    <mergeCell ref="L34:L35"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="H36:H37"/>
-    <mergeCell ref="I36:I37"/>
-    <mergeCell ref="J36:J37"/>
-    <mergeCell ref="K36:K37"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="G40:G42"/>
-    <mergeCell ref="H40:H42"/>
-    <mergeCell ref="I40:I42"/>
-    <mergeCell ref="J40:J42"/>
-    <mergeCell ref="K40:K42"/>
-    <mergeCell ref="L40:L42"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="K43:K44"/>
-    <mergeCell ref="L43:L44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="I43:I44"/>
-    <mergeCell ref="J43:J44"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="I45:I46"/>
-    <mergeCell ref="J45:J46"/>
-    <mergeCell ref="K45:K46"/>
-    <mergeCell ref="L45:L46"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="K47:K48"/>
-    <mergeCell ref="L47:L48"/>
-    <mergeCell ref="E49:E52"/>
-    <mergeCell ref="F49:F52"/>
-    <mergeCell ref="G49:G52"/>
-    <mergeCell ref="H49:H52"/>
-    <mergeCell ref="I49:I52"/>
-    <mergeCell ref="J49:J52"/>
-    <mergeCell ref="K49:K52"/>
-    <mergeCell ref="L49:L52"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="I47:I48"/>
-    <mergeCell ref="J47:J48"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="M40:M42"/>
-    <mergeCell ref="M43:M44"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="M47:M48"/>
-    <mergeCell ref="M49:M52"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="M17:M19"/>
-    <mergeCell ref="M20:M22"/>
-    <mergeCell ref="M23:M25"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="M28:M29"/>
-    <mergeCell ref="M30:M31"/>
-    <mergeCell ref="M32:M33"/>
-    <mergeCell ref="M34:M35"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="M2:M8"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="L17:L19"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="L2:L8"/>
+    <mergeCell ref="B26:B33"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B43:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B34:B42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="J2:J8"/>
+    <mergeCell ref="K2:K8"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="E2:E8"/>
+    <mergeCell ref="F2:F8"/>
+    <mergeCell ref="G2:G8"/>
+    <mergeCell ref="H2:H8"/>
+    <mergeCell ref="I2:I8"/>
+    <mergeCell ref="I11:I12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="https://drive.google.com/open?id=1RYgFxmL-dmZYtjF2ca5a0yQUWnMVjo3mVexJabJL1c4"/>
@@ -14862,10 +14862,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A2" s="282" t="s">
+      <c r="A2" s="281" t="s">
         <v>305</v>
       </c>
-      <c r="B2" s="277">
+      <c r="B2" s="274">
         <v>1</v>
       </c>
       <c r="C2" s="107">
@@ -14885,8 +14885,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A3" s="283"/>
-      <c r="B3" s="278"/>
+      <c r="A3" s="282"/>
+      <c r="B3" s="275"/>
       <c r="C3" s="107">
         <v>43193</v>
       </c>
@@ -14902,8 +14902,8 @@
       <c r="I3" s="112"/>
     </row>
     <row r="4" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A4" s="283"/>
-      <c r="B4" s="278"/>
+      <c r="A4" s="282"/>
+      <c r="B4" s="275"/>
       <c r="C4" s="107">
         <v>43194</v>
       </c>
@@ -14919,8 +14919,8 @@
       <c r="I4" s="112"/>
     </row>
     <row r="5" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A5" s="283"/>
-      <c r="B5" s="278"/>
+      <c r="A5" s="282"/>
+      <c r="B5" s="275"/>
       <c r="C5" s="107">
         <v>43195</v>
       </c>
@@ -14938,8 +14938,8 @@
       <c r="I5" s="112"/>
     </row>
     <row r="6" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A6" s="284"/>
-      <c r="B6" s="281"/>
+      <c r="A6" s="283"/>
+      <c r="B6" s="276"/>
       <c r="C6" s="114">
         <v>43196</v>
       </c>
@@ -14955,10 +14955,10 @@
       <c r="I6" s="118"/>
     </row>
     <row r="7" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A7" s="292" t="s">
+      <c r="A7" s="288" t="s">
         <v>184</v>
       </c>
-      <c r="B7" s="280">
+      <c r="B7" s="284">
         <v>2</v>
       </c>
       <c r="C7" s="140">
@@ -14976,8 +14976,8 @@
       <c r="I7" s="123"/>
     </row>
     <row r="8" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A8" s="293"/>
-      <c r="B8" s="275"/>
+      <c r="A8" s="289"/>
+      <c r="B8" s="285"/>
       <c r="C8" s="140">
         <v>43200</v>
       </c>
@@ -14993,8 +14993,8 @@
       <c r="I8" s="123"/>
     </row>
     <row r="9" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A9" s="293"/>
-      <c r="B9" s="275"/>
+      <c r="A9" s="289"/>
+      <c r="B9" s="285"/>
       <c r="C9" s="140">
         <v>43201</v>
       </c>
@@ -15010,8 +15010,8 @@
       <c r="I9" s="123"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A10" s="293"/>
-      <c r="B10" s="275"/>
+      <c r="A10" s="289"/>
+      <c r="B10" s="285"/>
       <c r="C10" s="140">
         <v>43202</v>
       </c>
@@ -15027,8 +15027,8 @@
       <c r="I10" s="123"/>
     </row>
     <row r="11" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A11" s="293"/>
-      <c r="B11" s="285"/>
+      <c r="A11" s="289"/>
+      <c r="B11" s="286"/>
       <c r="C11" s="140">
         <v>43203</v>
       </c>
@@ -15046,8 +15046,8 @@
       <c r="I11" s="123"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A12" s="272"/>
-      <c r="B12" s="286">
+      <c r="A12" s="290"/>
+      <c r="B12" s="280">
         <v>3</v>
       </c>
       <c r="C12" s="107">
@@ -15065,8 +15065,8 @@
       <c r="I12" s="112"/>
     </row>
     <row r="13" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A13" s="272"/>
-      <c r="B13" s="278"/>
+      <c r="A13" s="290"/>
+      <c r="B13" s="275"/>
       <c r="C13" s="107">
         <v>43207</v>
       </c>
@@ -15082,8 +15082,8 @@
       <c r="I13" s="112"/>
     </row>
     <row r="14" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A14" s="272"/>
-      <c r="B14" s="278"/>
+      <c r="A14" s="290"/>
+      <c r="B14" s="275"/>
       <c r="C14" s="107">
         <v>43208</v>
       </c>
@@ -15099,8 +15099,8 @@
       <c r="I14" s="112"/>
     </row>
     <row r="15" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A15" s="272"/>
-      <c r="B15" s="278"/>
+      <c r="A15" s="290"/>
+      <c r="B15" s="275"/>
       <c r="C15" s="107">
         <v>43209</v>
       </c>
@@ -15116,8 +15116,8 @@
       <c r="I15" s="112"/>
     </row>
     <row r="16" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A16" s="272"/>
-      <c r="B16" s="279"/>
+      <c r="A16" s="290"/>
+      <c r="B16" s="287"/>
       <c r="C16" s="107">
         <v>43210</v>
       </c>
@@ -15133,8 +15133,8 @@
       <c r="I16" s="112"/>
     </row>
     <row r="17" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A17" s="272"/>
-      <c r="B17" s="280">
+      <c r="A17" s="290"/>
+      <c r="B17" s="284">
         <v>4</v>
       </c>
       <c r="C17" s="119">
@@ -15156,8 +15156,8 @@
       <c r="I17" s="123"/>
     </row>
     <row r="18" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A18" s="272"/>
-      <c r="B18" s="275"/>
+      <c r="A18" s="290"/>
+      <c r="B18" s="285"/>
       <c r="C18" s="119">
         <v>43214</v>
       </c>
@@ -15173,8 +15173,8 @@
       <c r="I18" s="123"/>
     </row>
     <row r="19" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A19" s="272"/>
-      <c r="B19" s="275"/>
+      <c r="A19" s="290"/>
+      <c r="B19" s="285"/>
       <c r="C19" s="119">
         <v>43215</v>
       </c>
@@ -15190,8 +15190,8 @@
       <c r="I19" s="123"/>
     </row>
     <row r="20" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A20" s="272"/>
-      <c r="B20" s="275"/>
+      <c r="A20" s="290"/>
+      <c r="B20" s="285"/>
       <c r="C20" s="119">
         <v>43216</v>
       </c>
@@ -15207,8 +15207,8 @@
       <c r="I20" s="123"/>
     </row>
     <row r="21" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A21" s="272"/>
-      <c r="B21" s="285"/>
+      <c r="A21" s="290"/>
+      <c r="B21" s="286"/>
       <c r="C21" s="119">
         <v>43217</v>
       </c>
@@ -15226,8 +15226,8 @@
       <c r="I21" s="123"/>
     </row>
     <row r="22" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A22" s="272"/>
-      <c r="B22" s="286">
+      <c r="A22" s="290"/>
+      <c r="B22" s="280">
         <v>5</v>
       </c>
       <c r="C22" s="107">
@@ -15245,8 +15245,8 @@
       <c r="I22" s="112"/>
     </row>
     <row r="23" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A23" s="272"/>
-      <c r="B23" s="278"/>
+      <c r="A23" s="290"/>
+      <c r="B23" s="275"/>
       <c r="C23" s="107">
         <v>43221</v>
       </c>
@@ -15262,8 +15262,8 @@
       <c r="I23" s="112"/>
     </row>
     <row r="24" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A24" s="272"/>
-      <c r="B24" s="278"/>
+      <c r="A24" s="290"/>
+      <c r="B24" s="275"/>
       <c r="C24" s="107">
         <v>43222</v>
       </c>
@@ -15279,8 +15279,8 @@
       <c r="I24" s="112"/>
     </row>
     <row r="25" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A25" s="272"/>
-      <c r="B25" s="278"/>
+      <c r="A25" s="290"/>
+      <c r="B25" s="275"/>
       <c r="C25" s="107">
         <v>43223</v>
       </c>
@@ -15296,8 +15296,8 @@
       <c r="I25" s="112"/>
     </row>
     <row r="26" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A26" s="272"/>
-      <c r="B26" s="279"/>
+      <c r="A26" s="290"/>
+      <c r="B26" s="287"/>
       <c r="C26" s="107">
         <v>43224</v>
       </c>
@@ -15313,8 +15313,8 @@
       <c r="I26" s="112"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A27" s="272"/>
-      <c r="B27" s="290">
+      <c r="A27" s="290"/>
+      <c r="B27" s="292">
         <v>6</v>
       </c>
       <c r="C27" s="127">
@@ -15336,8 +15336,8 @@
       <c r="I27" s="123"/>
     </row>
     <row r="28" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A28" s="272"/>
-      <c r="B28" s="288"/>
+      <c r="A28" s="290"/>
+      <c r="B28" s="278"/>
       <c r="C28" s="127">
         <v>43228</v>
       </c>
@@ -15353,8 +15353,8 @@
       <c r="I28" s="123"/>
     </row>
     <row r="29" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A29" s="272"/>
-      <c r="B29" s="288"/>
+      <c r="A29" s="290"/>
+      <c r="B29" s="278"/>
       <c r="C29" s="127">
         <v>43229</v>
       </c>
@@ -15370,8 +15370,8 @@
       <c r="I29" s="123"/>
     </row>
     <row r="30" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A30" s="272"/>
-      <c r="B30" s="288"/>
+      <c r="A30" s="290"/>
+      <c r="B30" s="278"/>
       <c r="C30" s="127">
         <v>43230</v>
       </c>
@@ -15387,8 +15387,8 @@
       <c r="I30" s="123"/>
     </row>
     <row r="31" spans="1:9" ht="27" thickBot="1">
-      <c r="A31" s="273"/>
-      <c r="B31" s="291"/>
+      <c r="A31" s="291"/>
+      <c r="B31" s="293"/>
       <c r="C31" s="131">
         <v>43231</v>
       </c>
@@ -15406,10 +15406,10 @@
       <c r="I31" s="135"/>
     </row>
     <row r="32" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A32" s="282" t="s">
+      <c r="A32" s="281" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="277">
+      <c r="B32" s="274">
         <v>7</v>
       </c>
       <c r="C32" s="107">
@@ -15427,8 +15427,8 @@
       <c r="I32" s="112"/>
     </row>
     <row r="33" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A33" s="283"/>
-      <c r="B33" s="278"/>
+      <c r="A33" s="282"/>
+      <c r="B33" s="275"/>
       <c r="C33" s="107">
         <v>43235</v>
       </c>
@@ -15444,8 +15444,8 @@
       <c r="I33" s="112"/>
     </row>
     <row r="34" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A34" s="283"/>
-      <c r="B34" s="278"/>
+      <c r="A34" s="282"/>
+      <c r="B34" s="275"/>
       <c r="C34" s="107">
         <v>43236</v>
       </c>
@@ -15461,8 +15461,8 @@
       <c r="I34" s="112"/>
     </row>
     <row r="35" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A35" s="283"/>
-      <c r="B35" s="278"/>
+      <c r="A35" s="282"/>
+      <c r="B35" s="275"/>
       <c r="C35" s="107">
         <v>43237</v>
       </c>
@@ -15478,8 +15478,8 @@
       <c r="I35" s="112"/>
     </row>
     <row r="36" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A36" s="283"/>
-      <c r="B36" s="281"/>
+      <c r="A36" s="282"/>
+      <c r="B36" s="276"/>
       <c r="C36" s="107">
         <v>43238</v>
       </c>
@@ -15495,8 +15495,8 @@
       <c r="I36" s="112"/>
     </row>
     <row r="37" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A37" s="283"/>
-      <c r="B37" s="287">
+      <c r="A37" s="282"/>
+      <c r="B37" s="277">
         <v>8</v>
       </c>
       <c r="C37" s="127">
@@ -15518,8 +15518,8 @@
       <c r="I37" s="123"/>
     </row>
     <row r="38" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A38" s="283"/>
-      <c r="B38" s="288"/>
+      <c r="A38" s="282"/>
+      <c r="B38" s="278"/>
       <c r="C38" s="127">
         <v>43242</v>
       </c>
@@ -15535,8 +15535,8 @@
       <c r="I38" s="123"/>
     </row>
     <row r="39" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A39" s="283"/>
-      <c r="B39" s="288"/>
+      <c r="A39" s="282"/>
+      <c r="B39" s="278"/>
       <c r="C39" s="127">
         <v>43243</v>
       </c>
@@ -15552,8 +15552,8 @@
       <c r="I39" s="123"/>
     </row>
     <row r="40" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A40" s="283"/>
-      <c r="B40" s="288"/>
+      <c r="A40" s="282"/>
+      <c r="B40" s="278"/>
       <c r="C40" s="127">
         <v>43244</v>
       </c>
@@ -15569,8 +15569,8 @@
       <c r="I40" s="123"/>
     </row>
     <row r="41" spans="1:9" ht="27" thickBot="1">
-      <c r="A41" s="283"/>
-      <c r="B41" s="289"/>
+      <c r="A41" s="282"/>
+      <c r="B41" s="279"/>
       <c r="C41" s="127">
         <v>43245</v>
       </c>
@@ -15588,8 +15588,8 @@
       <c r="I41" s="123"/>
     </row>
     <row r="42" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A42" s="283"/>
-      <c r="B42" s="286">
+      <c r="A42" s="282"/>
+      <c r="B42" s="280">
         <v>9</v>
       </c>
       <c r="C42" s="107">
@@ -15607,8 +15607,8 @@
       <c r="I42" s="112"/>
     </row>
     <row r="43" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A43" s="283"/>
-      <c r="B43" s="278"/>
+      <c r="A43" s="282"/>
+      <c r="B43" s="275"/>
       <c r="C43" s="107">
         <v>43249</v>
       </c>
@@ -15624,8 +15624,8 @@
       <c r="I43" s="112"/>
     </row>
     <row r="44" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A44" s="283"/>
-      <c r="B44" s="278"/>
+      <c r="A44" s="282"/>
+      <c r="B44" s="275"/>
       <c r="C44" s="107">
         <v>43250</v>
       </c>
@@ -15641,8 +15641,8 @@
       <c r="I44" s="112"/>
     </row>
     <row r="45" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A45" s="283"/>
-      <c r="B45" s="278"/>
+      <c r="A45" s="282"/>
+      <c r="B45" s="275"/>
       <c r="C45" s="107">
         <v>43251</v>
       </c>
@@ -15658,8 +15658,8 @@
       <c r="I45" s="112"/>
     </row>
     <row r="46" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A46" s="284"/>
-      <c r="B46" s="281"/>
+      <c r="A46" s="283"/>
+      <c r="B46" s="276"/>
       <c r="C46" s="114">
         <v>43252</v>
       </c>
@@ -15675,10 +15675,10 @@
       <c r="I46" s="118"/>
     </row>
     <row r="47" spans="1:9" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A47" s="271" t="s">
+      <c r="A47" s="296" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="274">
+      <c r="B47" s="294">
         <v>10</v>
       </c>
       <c r="C47" s="119">
@@ -15700,8 +15700,8 @@
       <c r="I47" s="123"/>
     </row>
     <row r="48" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A48" s="272"/>
-      <c r="B48" s="275"/>
+      <c r="A48" s="290"/>
+      <c r="B48" s="285"/>
       <c r="C48" s="119">
         <v>43256</v>
       </c>
@@ -15717,8 +15717,8 @@
       <c r="I48" s="123"/>
     </row>
     <row r="49" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A49" s="272"/>
-      <c r="B49" s="275"/>
+      <c r="A49" s="290"/>
+      <c r="B49" s="285"/>
       <c r="C49" s="119">
         <v>43257</v>
       </c>
@@ -15734,8 +15734,8 @@
       <c r="I49" s="123"/>
     </row>
     <row r="50" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A50" s="272"/>
-      <c r="B50" s="275"/>
+      <c r="A50" s="290"/>
+      <c r="B50" s="285"/>
       <c r="C50" s="119">
         <v>43258</v>
       </c>
@@ -15751,8 +15751,8 @@
       <c r="I50" s="123"/>
     </row>
     <row r="51" spans="1:9" ht="27" thickBot="1">
-      <c r="A51" s="272"/>
-      <c r="B51" s="276"/>
+      <c r="A51" s="290"/>
+      <c r="B51" s="295"/>
       <c r="C51" s="119">
         <v>43259</v>
       </c>
@@ -15770,8 +15770,8 @@
       <c r="I51" s="123"/>
     </row>
     <row r="52" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A52" s="272"/>
-      <c r="B52" s="277">
+      <c r="A52" s="290"/>
+      <c r="B52" s="274">
         <v>11</v>
       </c>
       <c r="C52" s="107">
@@ -15789,8 +15789,8 @@
       <c r="I52" s="112"/>
     </row>
     <row r="53" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A53" s="272"/>
-      <c r="B53" s="278"/>
+      <c r="A53" s="290"/>
+      <c r="B53" s="275"/>
       <c r="C53" s="107">
         <v>43263</v>
       </c>
@@ -15806,8 +15806,8 @@
       <c r="I53" s="112"/>
     </row>
     <row r="54" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A54" s="272"/>
-      <c r="B54" s="278"/>
+      <c r="A54" s="290"/>
+      <c r="B54" s="275"/>
       <c r="C54" s="107">
         <v>43264</v>
       </c>
@@ -15823,8 +15823,8 @@
       <c r="I54" s="112"/>
     </row>
     <row r="55" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A55" s="272"/>
-      <c r="B55" s="278"/>
+      <c r="A55" s="290"/>
+      <c r="B55" s="275"/>
       <c r="C55" s="107">
         <v>43265</v>
       </c>
@@ -15840,8 +15840,8 @@
       <c r="I55" s="112"/>
     </row>
     <row r="56" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A56" s="272"/>
-      <c r="B56" s="279"/>
+      <c r="A56" s="290"/>
+      <c r="B56" s="287"/>
       <c r="C56" s="107">
         <v>43266</v>
       </c>
@@ -15857,8 +15857,8 @@
       <c r="I56" s="112"/>
     </row>
     <row r="57" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A57" s="272"/>
-      <c r="B57" s="280">
+      <c r="A57" s="290"/>
+      <c r="B57" s="284">
         <v>12</v>
       </c>
       <c r="C57" s="119">
@@ -15880,8 +15880,8 @@
       <c r="I57" s="123"/>
     </row>
     <row r="58" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A58" s="272"/>
-      <c r="B58" s="275"/>
+      <c r="A58" s="290"/>
+      <c r="B58" s="285"/>
       <c r="C58" s="119">
         <v>43270</v>
       </c>
@@ -15897,8 +15897,8 @@
       <c r="I58" s="123"/>
     </row>
     <row r="59" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A59" s="272"/>
-      <c r="B59" s="275"/>
+      <c r="A59" s="290"/>
+      <c r="B59" s="285"/>
       <c r="C59" s="119">
         <v>43271</v>
       </c>
@@ -15914,8 +15914,8 @@
       <c r="I59" s="123"/>
     </row>
     <row r="60" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A60" s="272"/>
-      <c r="B60" s="275"/>
+      <c r="A60" s="290"/>
+      <c r="B60" s="285"/>
       <c r="C60" s="119">
         <v>43272</v>
       </c>
@@ -15931,8 +15931,8 @@
       <c r="I60" s="123"/>
     </row>
     <row r="61" spans="1:9" ht="27" thickBot="1">
-      <c r="A61" s="273"/>
-      <c r="B61" s="276"/>
+      <c r="A61" s="291"/>
+      <c r="B61" s="295"/>
       <c r="C61" s="137">
         <v>43273</v>
       </c>
@@ -15950,10 +15950,10 @@
       <c r="I61" s="135"/>
     </row>
     <row r="62" spans="1:9" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A62" s="282" t="s">
+      <c r="A62" s="281" t="s">
         <v>627</v>
       </c>
-      <c r="B62" s="277">
+      <c r="B62" s="274">
         <v>13</v>
       </c>
       <c r="C62" s="107">
@@ -15971,8 +15971,8 @@
       <c r="I62" s="112"/>
     </row>
     <row r="63" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A63" s="283"/>
-      <c r="B63" s="278"/>
+      <c r="A63" s="282"/>
+      <c r="B63" s="275"/>
       <c r="C63" s="107">
         <v>43277</v>
       </c>
@@ -15988,8 +15988,8 @@
       <c r="I63" s="112"/>
     </row>
     <row r="64" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A64" s="283"/>
-      <c r="B64" s="278"/>
+      <c r="A64" s="282"/>
+      <c r="B64" s="275"/>
       <c r="C64" s="107">
         <v>43278</v>
       </c>
@@ -16005,8 +16005,8 @@
       <c r="I64" s="112"/>
     </row>
     <row r="65" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A65" s="283"/>
-      <c r="B65" s="278"/>
+      <c r="A65" s="282"/>
+      <c r="B65" s="275"/>
       <c r="C65" s="107">
         <v>43279</v>
       </c>
@@ -16022,8 +16022,8 @@
       <c r="I65" s="112"/>
     </row>
     <row r="66" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A66" s="283"/>
-      <c r="B66" s="281"/>
+      <c r="A66" s="282"/>
+      <c r="B66" s="276"/>
       <c r="C66" s="107">
         <v>43280</v>
       </c>
@@ -16039,8 +16039,8 @@
       <c r="I66" s="112"/>
     </row>
     <row r="67" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A67" s="283"/>
-      <c r="B67" s="287">
+      <c r="A67" s="282"/>
+      <c r="B67" s="277">
         <v>14</v>
       </c>
       <c r="C67" s="127">
@@ -16062,8 +16062,8 @@
       <c r="I67" s="123"/>
     </row>
     <row r="68" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A68" s="283"/>
-      <c r="B68" s="288"/>
+      <c r="A68" s="282"/>
+      <c r="B68" s="278"/>
       <c r="C68" s="127">
         <v>43284</v>
       </c>
@@ -16079,8 +16079,8 @@
       <c r="I68" s="123"/>
     </row>
     <row r="69" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A69" s="283"/>
-      <c r="B69" s="288"/>
+      <c r="A69" s="282"/>
+      <c r="B69" s="278"/>
       <c r="C69" s="127">
         <v>43285</v>
       </c>
@@ -16096,8 +16096,8 @@
       <c r="I69" s="123"/>
     </row>
     <row r="70" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A70" s="283"/>
-      <c r="B70" s="288"/>
+      <c r="A70" s="282"/>
+      <c r="B70" s="278"/>
       <c r="C70" s="127">
         <v>43286</v>
       </c>
@@ -16113,8 +16113,8 @@
       <c r="I70" s="123"/>
     </row>
     <row r="71" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A71" s="283"/>
-      <c r="B71" s="289"/>
+      <c r="A71" s="282"/>
+      <c r="B71" s="279"/>
       <c r="C71" s="127">
         <v>43287</v>
       </c>
@@ -16132,8 +16132,8 @@
       <c r="I71" s="123"/>
     </row>
     <row r="72" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A72" s="283"/>
-      <c r="B72" s="286">
+      <c r="A72" s="282"/>
+      <c r="B72" s="280">
         <v>15</v>
       </c>
       <c r="C72" s="107">
@@ -16151,8 +16151,8 @@
       <c r="I72" s="112"/>
     </row>
     <row r="73" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A73" s="283"/>
-      <c r="B73" s="278"/>
+      <c r="A73" s="282"/>
+      <c r="B73" s="275"/>
       <c r="C73" s="107">
         <v>43291</v>
       </c>
@@ -16168,8 +16168,8 @@
       <c r="I73" s="112"/>
     </row>
     <row r="74" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A74" s="283"/>
-      <c r="B74" s="278"/>
+      <c r="A74" s="282"/>
+      <c r="B74" s="275"/>
       <c r="C74" s="107">
         <v>43292</v>
       </c>
@@ -16185,8 +16185,8 @@
       <c r="I74" s="112"/>
     </row>
     <row r="75" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A75" s="283"/>
-      <c r="B75" s="278"/>
+      <c r="A75" s="282"/>
+      <c r="B75" s="275"/>
       <c r="C75" s="107">
         <v>43293</v>
       </c>
@@ -16202,8 +16202,8 @@
       <c r="I75" s="112"/>
     </row>
     <row r="76" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A76" s="283"/>
-      <c r="B76" s="279"/>
+      <c r="A76" s="282"/>
+      <c r="B76" s="287"/>
       <c r="C76" s="107">
         <v>43294</v>
       </c>
@@ -16219,8 +16219,8 @@
       <c r="I76" s="112"/>
     </row>
     <row r="77" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A77" s="283"/>
-      <c r="B77" s="290">
+      <c r="A77" s="282"/>
+      <c r="B77" s="292">
         <v>16</v>
       </c>
       <c r="C77" s="127">
@@ -16242,8 +16242,8 @@
       <c r="I77" s="123"/>
     </row>
     <row r="78" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A78" s="283"/>
-      <c r="B78" s="288"/>
+      <c r="A78" s="282"/>
+      <c r="B78" s="278"/>
       <c r="C78" s="127">
         <v>43298</v>
       </c>
@@ -16259,8 +16259,8 @@
       <c r="I78" s="123"/>
     </row>
     <row r="79" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A79" s="283"/>
-      <c r="B79" s="288"/>
+      <c r="A79" s="282"/>
+      <c r="B79" s="278"/>
       <c r="C79" s="127">
         <v>43299</v>
       </c>
@@ -16276,8 +16276,8 @@
       <c r="I79" s="123"/>
     </row>
     <row r="80" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A80" s="283"/>
-      <c r="B80" s="288"/>
+      <c r="A80" s="282"/>
+      <c r="B80" s="278"/>
       <c r="C80" s="127">
         <v>43300</v>
       </c>
@@ -16293,8 +16293,8 @@
       <c r="I80" s="123"/>
     </row>
     <row r="81" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A81" s="284"/>
-      <c r="B81" s="291"/>
+      <c r="A81" s="283"/>
+      <c r="B81" s="293"/>
       <c r="C81" s="131">
         <v>43301</v>
       </c>
@@ -16312,10 +16312,10 @@
       <c r="I81" s="135"/>
     </row>
     <row r="82" spans="1:9" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A82" s="282" t="s">
+      <c r="A82" s="281" t="s">
         <v>76</v>
       </c>
-      <c r="B82" s="277">
+      <c r="B82" s="274">
         <v>17</v>
       </c>
       <c r="C82" s="107">
@@ -16333,8 +16333,8 @@
       <c r="I82" s="112"/>
     </row>
     <row r="83" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A83" s="283"/>
-      <c r="B83" s="278"/>
+      <c r="A83" s="282"/>
+      <c r="B83" s="275"/>
       <c r="C83" s="107">
         <v>43305</v>
       </c>
@@ -16350,8 +16350,8 @@
       <c r="I83" s="112"/>
     </row>
     <row r="84" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A84" s="283"/>
-      <c r="B84" s="278"/>
+      <c r="A84" s="282"/>
+      <c r="B84" s="275"/>
       <c r="C84" s="107">
         <v>43306</v>
       </c>
@@ -16367,8 +16367,8 @@
       <c r="I84" s="112"/>
     </row>
     <row r="85" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A85" s="283"/>
-      <c r="B85" s="278"/>
+      <c r="A85" s="282"/>
+      <c r="B85" s="275"/>
       <c r="C85" s="107">
         <v>43307</v>
       </c>
@@ -16384,8 +16384,8 @@
       <c r="I85" s="112"/>
     </row>
     <row r="86" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A86" s="284"/>
-      <c r="B86" s="281"/>
+      <c r="A86" s="283"/>
+      <c r="B86" s="276"/>
       <c r="C86" s="114">
         <v>43308</v>
       </c>
@@ -16401,10 +16401,10 @@
       <c r="I86" s="118"/>
     </row>
     <row r="87" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A87" s="282" t="s">
+      <c r="A87" s="281" t="s">
         <v>632</v>
       </c>
-      <c r="B87" s="274">
+      <c r="B87" s="294">
         <v>18</v>
       </c>
       <c r="C87" s="119">
@@ -16426,8 +16426,8 @@
       <c r="I87" s="123"/>
     </row>
     <row r="88" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A88" s="283"/>
-      <c r="B88" s="275"/>
+      <c r="A88" s="282"/>
+      <c r="B88" s="285"/>
       <c r="C88" s="119">
         <v>43312</v>
       </c>
@@ -16443,8 +16443,8 @@
       <c r="I88" s="123"/>
     </row>
     <row r="89" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A89" s="283"/>
-      <c r="B89" s="275"/>
+      <c r="A89" s="282"/>
+      <c r="B89" s="285"/>
       <c r="C89" s="119">
         <v>43313</v>
       </c>
@@ -16460,8 +16460,8 @@
       <c r="I89" s="123"/>
     </row>
     <row r="90" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A90" s="283"/>
-      <c r="B90" s="275"/>
+      <c r="A90" s="282"/>
+      <c r="B90" s="285"/>
       <c r="C90" s="119">
         <v>43314</v>
       </c>
@@ -16477,8 +16477,8 @@
       <c r="I90" s="123"/>
     </row>
     <row r="91" spans="1:9" ht="27" thickBot="1">
-      <c r="A91" s="283"/>
-      <c r="B91" s="285"/>
+      <c r="A91" s="282"/>
+      <c r="B91" s="286"/>
       <c r="C91" s="119">
         <v>43315</v>
       </c>
@@ -16496,8 +16496,8 @@
       <c r="I91" s="123"/>
     </row>
     <row r="92" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A92" s="283"/>
-      <c r="B92" s="286">
+      <c r="A92" s="282"/>
+      <c r="B92" s="280">
         <v>19</v>
       </c>
       <c r="C92" s="107">
@@ -16515,8 +16515,8 @@
       <c r="I92" s="112"/>
     </row>
     <row r="93" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A93" s="283"/>
-      <c r="B93" s="278"/>
+      <c r="A93" s="282"/>
+      <c r="B93" s="275"/>
       <c r="C93" s="107">
         <v>43319</v>
       </c>
@@ -16532,8 +16532,8 @@
       <c r="I93" s="112"/>
     </row>
     <row r="94" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A94" s="283"/>
-      <c r="B94" s="278"/>
+      <c r="A94" s="282"/>
+      <c r="B94" s="275"/>
       <c r="C94" s="107">
         <v>43320</v>
       </c>
@@ -16549,8 +16549,8 @@
       <c r="I94" s="112"/>
     </row>
     <row r="95" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A95" s="283"/>
-      <c r="B95" s="278"/>
+      <c r="A95" s="282"/>
+      <c r="B95" s="275"/>
       <c r="C95" s="107">
         <v>43321</v>
       </c>
@@ -16566,8 +16566,8 @@
       <c r="I95" s="112"/>
     </row>
     <row r="96" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A96" s="283"/>
-      <c r="B96" s="279"/>
+      <c r="A96" s="282"/>
+      <c r="B96" s="287"/>
       <c r="C96" s="107">
         <v>43322</v>
       </c>
@@ -16583,8 +16583,8 @@
       <c r="I96" s="112"/>
     </row>
     <row r="97" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A97" s="283"/>
-      <c r="B97" s="280">
+      <c r="A97" s="282"/>
+      <c r="B97" s="284">
         <v>20</v>
       </c>
       <c r="C97" s="119">
@@ -16604,8 +16604,8 @@
       <c r="I97" s="123"/>
     </row>
     <row r="98" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A98" s="283"/>
-      <c r="B98" s="275"/>
+      <c r="A98" s="282"/>
+      <c r="B98" s="285"/>
       <c r="C98" s="119">
         <v>43326</v>
       </c>
@@ -16621,8 +16621,8 @@
       <c r="I98" s="123"/>
     </row>
     <row r="99" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A99" s="283"/>
-      <c r="B99" s="275"/>
+      <c r="A99" s="282"/>
+      <c r="B99" s="285"/>
       <c r="C99" s="119">
         <v>43327</v>
       </c>
@@ -16638,8 +16638,8 @@
       <c r="I99" s="123"/>
     </row>
     <row r="100" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A100" s="283"/>
-      <c r="B100" s="275"/>
+      <c r="A100" s="282"/>
+      <c r="B100" s="285"/>
       <c r="C100" s="119">
         <v>43328</v>
       </c>
@@ -16657,8 +16657,8 @@
       <c r="I100" s="123"/>
     </row>
     <row r="101" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A101" s="284"/>
-      <c r="B101" s="276"/>
+      <c r="A101" s="283"/>
+      <c r="B101" s="295"/>
       <c r="C101" s="137">
         <v>43329</v>
       </c>
@@ -22968,6 +22968,21 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A47:A61"/>
+    <mergeCell ref="B47:B51"/>
+    <mergeCell ref="B52:B56"/>
+    <mergeCell ref="B57:B61"/>
+    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="A87:A101"/>
+    <mergeCell ref="A62:A81"/>
+    <mergeCell ref="B87:B91"/>
+    <mergeCell ref="B92:B96"/>
+    <mergeCell ref="B97:B101"/>
+    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="B72:B76"/>
+    <mergeCell ref="B77:B81"/>
+    <mergeCell ref="B82:B86"/>
     <mergeCell ref="B32:B36"/>
     <mergeCell ref="B37:B41"/>
     <mergeCell ref="B42:B46"/>
@@ -22980,21 +22995,6 @@
     <mergeCell ref="B22:B26"/>
     <mergeCell ref="B27:B31"/>
     <mergeCell ref="A32:A46"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="A87:A101"/>
-    <mergeCell ref="A62:A81"/>
-    <mergeCell ref="B87:B91"/>
-    <mergeCell ref="B92:B96"/>
-    <mergeCell ref="B97:B101"/>
-    <mergeCell ref="B67:B71"/>
-    <mergeCell ref="B72:B76"/>
-    <mergeCell ref="B77:B81"/>
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="A47:A61"/>
-    <mergeCell ref="B47:B51"/>
-    <mergeCell ref="B52:B56"/>
-    <mergeCell ref="B57:B61"/>
-    <mergeCell ref="B62:B66"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://drive.google.com/open?id=12f1t9Kg0CD9OW5iG5jB3Ozx_iRGw-cbyozVUPhhG6ME"/>
@@ -23010,7 +23010,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -23172,7 +23172,7 @@
       </c>
       <c r="D12" s="147">
         <f>SUM(D13:D20)</f>
-        <v>8.9700000000000002E-2</v>
+        <v>0.1173</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75">
@@ -23230,7 +23230,10 @@
       <c r="C16" s="80">
         <v>0.03</v>
       </c>
-      <c r="D16" s="57"/>
+      <c r="D16" s="57">
+        <f>C16*(0.82+0.1)</f>
+        <v>2.7599999999999996E-2</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="15.75">
       <c r="A17" s="56" t="s">
@@ -23281,16 +23284,16 @@
       <c r="D20" s="57"/>
     </row>
     <row r="21" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A21" s="300" t="s">
+      <c r="A21" s="190" t="s">
         <v>1002</v>
       </c>
-      <c r="B21" s="301">
+      <c r="B21" s="191">
         <v>43315</v>
       </c>
       <c r="C21" s="80">
         <v>0.03</v>
       </c>
-      <c r="D21" s="302"/>
+      <c r="D21" s="192"/>
     </row>
     <row r="22" spans="1:4" ht="16.5" thickBot="1">
       <c r="A22" s="62" t="s">
@@ -23414,7 +23417,7 @@
       </c>
       <c r="D32" s="67">
         <f>SUM(D2,D12,D22,D27,D28)</f>
-        <v>0.21970000000000001</v>
+        <v>0.24730000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -23475,11 +23478,11 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="C13" s="294" t="s">
+      <c r="C13" s="297" t="s">
         <v>168</v>
       </c>
-      <c r="D13" s="295"/>
-      <c r="E13" s="296"/>
+      <c r="D13" s="298"/>
+      <c r="E13" s="299"/>
     </row>
     <row r="14" spans="1:10">
       <c r="C14" t="s">
@@ -23495,16 +23498,16 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="294" t="s">
+      <c r="A16" s="297" t="s">
         <v>171</v>
       </c>
-      <c r="B16" s="295"/>
-      <c r="C16" s="296"/>
-      <c r="E16" s="294" t="s">
+      <c r="B16" s="298"/>
+      <c r="C16" s="299"/>
+      <c r="E16" s="297" t="s">
         <v>167</v>
       </c>
-      <c r="F16" s="295"/>
-      <c r="G16" s="296"/>
+      <c r="F16" s="298"/>
+      <c r="G16" s="299"/>
     </row>
     <row r="18" spans="1:6">
       <c r="B18" t="s">
@@ -23515,11 +23518,11 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="C19" s="294" t="s">
+      <c r="C19" s="297" t="s">
         <v>166</v>
       </c>
-      <c r="D19" s="295"/>
-      <c r="E19" s="296"/>
+      <c r="D19" s="298"/>
+      <c r="E19" s="299"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
@@ -25760,21 +25763,21 @@
     </row>
     <row r="319" spans="1:11" ht="15.75" thickBot="1"/>
     <row r="320" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A320" s="297" t="s">
+      <c r="A320" s="300" t="s">
         <v>243</v>
       </c>
-      <c r="B320" s="298"/>
-      <c r="C320" s="299"/>
-      <c r="E320" s="297" t="s">
+      <c r="B320" s="301"/>
+      <c r="C320" s="302"/>
+      <c r="E320" s="300" t="s">
         <v>249</v>
       </c>
-      <c r="F320" s="298"/>
-      <c r="G320" s="299"/>
-      <c r="I320" s="297" t="s">
+      <c r="F320" s="301"/>
+      <c r="G320" s="302"/>
+      <c r="I320" s="300" t="s">
         <v>946</v>
       </c>
-      <c r="J320" s="298"/>
-      <c r="K320" s="299"/>
+      <c r="J320" s="301"/>
+      <c r="K320" s="302"/>
     </row>
     <row r="321" spans="1:11" ht="15.75" thickBot="1">
       <c r="A321" s="152" t="s">

</xml_diff>